<commit_message>
Portfolio fixes with YTM/DUR
</commit_message>
<xml_diff>
--- a/models/Data.xlsx
+++ b/models/Data.xlsx
@@ -3,14 +3,8 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericl\go\src\OGN\models\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E2F0E1-D1BC-43D0-9EEC-DBDDDD74F910}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowHeight="32040" windowWidth="57840" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -33,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="143">
   <si>
     <t>RETT</t>
   </si>
@@ -459,18 +453,21 @@
   </si>
   <si>
     <t>Fit Out costs</t>
+  </si>
+  <si>
+    <t>OGANITA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0.0000_);_(* \(#,##0.0000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -661,19 +658,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="4" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
+        <fgColor theme="4" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -684,19 +681,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
+        <fgColor theme="5" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
+        <fgColor theme="5" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.39997558519241921"/>
+        <fgColor theme="5" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -707,19 +704,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.79998168889431442"/>
+        <fgColor theme="6" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="6" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -730,19 +727,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor theme="7" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor theme="7" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39997558519241921"/>
+        <fgColor theme="7" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -753,19 +750,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="8" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -776,19 +773,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
+        <fgColor theme="9" tint="0.7999816888943144"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.5999938962981048"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
+        <fgColor theme="9" tint="0.3999755851924192"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -824,7 +821,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.39997558519241921"/>
+        <color theme="4" tint="0.3999755851924192"/>
       </bottom>
       <diagonal/>
     </border>
@@ -911,114 +908,114 @@
   </borders>
   <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="true" applyAlignment="true">
+      <alignment wrapText="true"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="true" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="true" applyFont="true" applyAlignment="true">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center" vertical="center" wrapText="true"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="true"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="true"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="true"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="true"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="true"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="true"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="true"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="true"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="true"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="true"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="true"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="true"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="true"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="true"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="true"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="true"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="true"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="true"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="true"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="true"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="true"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="true"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="true"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="true"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="true"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="true"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="true"/>
     <cellStyle name="Comma" xfId="42" builtinId="3"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="true"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="true"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="true"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="true"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="true"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="true"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="true"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="true"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="true"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="true"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="true"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="true"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="true"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1329,73 +1326,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="3" topLeftCell="AK1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="AZ14" sqref="AZ14"/>
+    <sheetView tabSelected="true" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane activePane="topRight" state="frozen" topLeftCell="D1" xSplit="3"/>
+      <selection activeCell="G16" pane="topRight" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="5.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="20.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="11.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="5.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="11" style="4" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="10" style="4" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="12" style="4" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="19.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="9.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="8.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="11.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="18.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="14" style="4" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="14.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="14.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8" style="4" bestFit="1" customWidth="1"/>
-    <col min="55" max="56" width="10.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="6.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="58" max="16384" width="12.5703125" style="4"/>
+    <col bestFit="true" customWidth="true" max="1" min="1" style="4" width="5.140625"/>
+    <col bestFit="true" customWidth="true" max="2" min="2" style="4" width="9.140625"/>
+    <col bestFit="true" customWidth="true" max="3" min="3" style="4" width="15.7109375"/>
+    <col bestFit="true" customWidth="true" max="4" min="4" style="4" width="8.42578125"/>
+    <col bestFit="true" customWidth="true" max="5" min="5" style="4" width="12.140625"/>
+    <col bestFit="true" customWidth="true" max="6" min="6" style="4" width="11.7109375"/>
+    <col customWidth="true" max="7" min="7" style="4" width="12.42578125"/>
+    <col bestFit="true" customWidth="true" max="8" min="8" style="4" width="11.7109375"/>
+    <col bestFit="true" customWidth="true" max="9" min="9" style="4" width="10"/>
+    <col bestFit="true" customWidth="true" max="10" min="10" style="4" width="11.7109375"/>
+    <col bestFit="true" customWidth="true" max="11" min="11" style="4" width="18.28515625"/>
+    <col bestFit="true" customWidth="true" max="12" min="12" style="4" width="14.5703125"/>
+    <col bestFit="true" customWidth="true" max="13" min="13" style="4" width="18.7109375"/>
+    <col bestFit="true" customWidth="true" max="14" min="14" style="4" width="8.85546875"/>
+    <col bestFit="true" customWidth="true" max="15" min="15" style="4" width="17.7109375"/>
+    <col bestFit="true" customWidth="true" max="16" min="16" style="4" width="20.28515625"/>
+    <col bestFit="true" customWidth="true" max="17" min="17" style="4" width="13.28515625"/>
+    <col bestFit="true" customWidth="true" max="18" min="18" style="4" width="13.85546875"/>
+    <col bestFit="true" customWidth="true" max="19" min="19" style="4" width="10.5703125"/>
+    <col bestFit="true" customWidth="true" max="20" min="20" style="4" width="11"/>
+    <col bestFit="true" customWidth="true" max="21" min="21" style="4" width="9.28515625"/>
+    <col bestFit="true" customWidth="true" max="22" min="22" style="4" width="11.42578125"/>
+    <col bestFit="true" customWidth="true" max="23" min="23" style="4" width="5.5703125"/>
+    <col bestFit="true" customWidth="true" max="24" min="24" style="4" width="5.140625"/>
+    <col bestFit="true" customWidth="true" max="25" min="25" style="4" width="13.7109375"/>
+    <col bestFit="true" customWidth="true" max="26" min="26" style="4" width="11.7109375"/>
+    <col bestFit="true" customWidth="true" max="27" min="27" style="4" width="11"/>
+    <col bestFit="true" customWidth="true" max="28" min="28" style="4" width="8"/>
+    <col bestFit="true" customWidth="true" max="29" min="29" style="4" width="10"/>
+    <col bestFit="true" customWidth="true" max="30" min="30" style="4" width="14.140625"/>
+    <col bestFit="true" customWidth="true" max="31" min="31" style="4" width="12"/>
+    <col bestFit="true" customWidth="true" max="32" min="32" style="4" width="14.5703125"/>
+    <col bestFit="true" customWidth="true" max="33" min="33" style="4" width="19.5703125"/>
+    <col bestFit="true" customWidth="true" max="34" min="34" style="4" width="10.28515625"/>
+    <col bestFit="true" customWidth="true" max="35" min="35" style="4" width="8"/>
+    <col bestFit="true" customWidth="true" max="36" min="36" style="4" width="12.42578125"/>
+    <col bestFit="true" customWidth="true" max="37" min="37" style="4" width="9.140625"/>
+    <col bestFit="true" customWidth="true" max="38" min="38" style="4" width="10.140625"/>
+    <col bestFit="true" customWidth="true" max="39" min="39" style="4" width="16.140625"/>
+    <col bestFit="true" customWidth="true" max="40" min="40" style="4" width="8"/>
+    <col bestFit="true" customWidth="true" max="41" min="41" style="4" width="8.140625"/>
+    <col bestFit="true" customWidth="true" max="42" min="42" style="4" width="9.85546875"/>
+    <col bestFit="true" customWidth="true" max="43" min="43" style="4" width="8"/>
+    <col bestFit="true" customWidth="true" max="44" min="44" style="4" width="11.140625"/>
+    <col bestFit="true" customWidth="true" max="45" min="45" style="4" width="8"/>
+    <col bestFit="true" customWidth="true" max="46" min="46" style="4" width="18.28515625"/>
+    <col bestFit="true" customWidth="true" max="47" min="47" style="4" width="14.5703125"/>
+    <col bestFit="true" customWidth="true" max="48" min="48" style="4" width="13.7109375"/>
+    <col bestFit="true" customWidth="true" max="49" min="49" style="4" width="14"/>
+    <col bestFit="true" customWidth="true" max="50" min="50" style="4" width="14.7109375"/>
+    <col bestFit="true" customWidth="true" max="51" min="51" style="4" width="15.140625"/>
+    <col bestFit="true" customWidth="true" max="52" min="52" style="4" width="14.28515625"/>
+    <col bestFit="true" customWidth="true" max="53" min="53" style="4" width="14.5703125"/>
+    <col bestFit="true" customWidth="true" max="54" min="54" style="4" width="8"/>
+    <col bestFit="true" customWidth="true" max="56" min="55" style="4" width="10.5703125"/>
+    <col bestFit="true" customWidth="true" max="57" min="57" style="4" width="6.28515625"/>
+    <col max="16384" min="58" style="4" width="12.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:58" s="3" customFormat="true">
       <c r="A1" s="3">
         <v>0</v>
       </c>
@@ -1571,7 +1568,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="2" spans="1:58" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:58" s="5" customFormat="true" ht="45">
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1744,7 +1741,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="3" spans="1:58" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:58" s="5" customFormat="true">
       <c r="B3" s="5">
         <v>0</v>
       </c>
@@ -1770,131 +1767,135 @@
         <v>0</v>
       </c>
       <c r="K3" s="4">
-        <v>0</v>
+        <v>0.055</v>
       </c>
       <c r="L3" s="4">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="M3" s="4">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="N3" s="4">
-        <v>0</v>
+        <v>0.019</v>
       </c>
       <c r="O3" s="4">
-        <v>0</v>
+        <v>0.016</v>
       </c>
       <c r="P3" s="4">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="Q3" s="4">
-        <v>0</v>
+        <v>36</v>
       </c>
       <c r="R3" s="4">
-        <v>0</v>
+        <v>0.013000000000000001</v>
       </c>
       <c r="S3" s="4">
-        <v>0</v>
+        <v>0.0825</v>
       </c>
       <c r="T3" s="4">
-        <v>0</v>
+        <v>3.5</v>
       </c>
       <c r="U3" s="4"/>
       <c r="V3" s="4">
+        <v>15</v>
+      </c>
+      <c r="W3" s="4">
+        <v>0</v>
+      </c>
+      <c r="X3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="4">
+        <v>39</v>
+      </c>
+      <c r="AA3" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="AB3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="4">
+        <v>0.06</v>
+      </c>
+      <c r="AE3" s="4">
         <v>10</v>
       </c>
-      <c r="W3" s="4">
-        <v>0</v>
-      </c>
-      <c r="X3" s="4">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="4">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="4"/>
-      <c r="AA3" s="4">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="4">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="4">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="4">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="4">
-        <v>0</v>
-      </c>
       <c r="AF3" s="4">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AG3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH3" s="4" t="s">
-        <v>59</v>
+        <v>113</v>
       </c>
       <c r="AI3" s="4">
         <v>0</v>
       </c>
       <c r="AJ3" s="4">
-        <v>0</v>
+        <v>0.013999999999999999</v>
       </c>
       <c r="AK3" s="4">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="AL3" s="4">
-        <v>0</v>
+        <v>180</v>
       </c>
       <c r="AM3" s="4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN3" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AO3" s="4">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="AP3" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AQ3" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AR3" s="4">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="AS3" s="4">
-        <v>0</v>
+        <v>0.0075</v>
       </c>
       <c r="AT3" s="4">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="AU3" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AV3" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AW3" s="4">
-        <v>0</v>
+        <v>0.0025</v>
       </c>
       <c r="AX3" s="4">
-        <v>0</v>
+        <v>0.012</v>
       </c>
       <c r="AY3" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AZ3" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BA3" s="4">
-        <v>0</v>
-      </c>
-      <c r="BB3" s="4"/>
+        <v>0.0025</v>
+      </c>
+      <c r="BB3" s="4">
+        <v>0.0005</v>
+      </c>
       <c r="BC3" s="4">
         <v>0</v>
       </c>
@@ -1902,10 +1903,10 @@
         <v>0</v>
       </c>
       <c r="BF3" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:58" x14ac:dyDescent="0.25">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:58">
       <c r="B4" s="4">
         <v>3</v>
       </c>
@@ -2069,16 +2070,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:58">
       <c r="B5" s="4">
         <v>6</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D5" s="5">
-        <v>0</v>
-      </c>
+      <c r="D5" s="5"/>
       <c r="E5" s="4">
         <v>1</v>
       </c>
@@ -2233,7 +2232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:58">
       <c r="B6" s="4">
         <v>1</v>
       </c>
@@ -2262,34 +2261,34 @@
         <v>2035</v>
       </c>
       <c r="K6" s="4">
-        <v>5.7800000000000004E-2</v>
+        <v>0.06</v>
       </c>
       <c r="L6" s="4">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="M6" s="4">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="N6" s="4">
-        <v>1.83E-2</v>
+        <v>0.0148</v>
       </c>
       <c r="O6" s="4">
-        <v>4.2800000000000005E-2</v>
+        <v>0.0443</v>
       </c>
       <c r="P6" s="4">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="Q6" s="4">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="R6" s="4">
-        <v>2.1299999999999999E-2</v>
+        <v>0.024300000000000002</v>
       </c>
       <c r="S6" s="4">
-        <v>5.5500000000000001E-2</v>
+        <v>0.0555</v>
       </c>
       <c r="T6" s="4">
-        <v>3.2</v>
+        <v>4.86</v>
       </c>
       <c r="V6" s="4">
         <v>10</v>
@@ -2313,10 +2312,10 @@
         <v>0.6</v>
       </c>
       <c r="AC6" s="4">
-        <v>2.1000000000000001E-2</v>
+        <v>0.021</v>
       </c>
       <c r="AD6" s="4">
-        <v>0.22</v>
+        <v>0.2335</v>
       </c>
       <c r="AE6" s="4">
         <v>10</v>
@@ -2337,7 +2336,7 @@
         <v>0</v>
       </c>
       <c r="AK6" s="4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="AL6" s="4">
         <v>60</v>
@@ -2346,25 +2345,25 @@
         <v>1</v>
       </c>
       <c r="AN6" s="4">
-        <v>0.6765000000000001</v>
+        <v>0.6751999999999999</v>
       </c>
       <c r="AO6" s="4">
         <v>0</v>
       </c>
       <c r="AP6" s="4">
-        <v>2.1</v>
+        <v>2.2</v>
       </c>
       <c r="AQ6" s="4">
-        <v>1.2</v>
+        <v>2</v>
       </c>
       <c r="AR6" s="4">
-        <v>2.1499999999999998E-2</v>
+        <v>0.0345</v>
       </c>
       <c r="AS6" s="4">
-        <v>0.02</v>
+        <v>0.035</v>
       </c>
       <c r="AT6" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.0085</v>
       </c>
       <c r="AU6" s="4">
         <v>6</v>
@@ -2373,10 +2372,10 @@
         <v>6</v>
       </c>
       <c r="AW6" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.001</v>
       </c>
       <c r="AX6" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.0085</v>
       </c>
       <c r="AY6" s="4">
         <v>6</v>
@@ -2385,10 +2384,10 @@
         <v>6</v>
       </c>
       <c r="BA6" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.001</v>
       </c>
       <c r="BB6" s="4">
-        <v>4.0000000000000001E-3</v>
+        <v>0.004</v>
       </c>
       <c r="BC6" s="4">
         <v>3</v>
@@ -2403,7 +2402,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:58">
       <c r="B7" s="4">
         <v>4</v>
       </c>
@@ -2432,7 +2431,7 @@
         <v>2035</v>
       </c>
       <c r="K7" s="4">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="L7" s="4">
         <v>18</v>
@@ -2441,10 +2440,10 @@
         <v>18</v>
       </c>
       <c r="N7" s="4">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="O7" s="4">
-        <v>2.8500000000000001E-2</v>
+        <v>0.0285</v>
       </c>
       <c r="P7" s="4">
         <v>36</v>
@@ -2453,10 +2452,10 @@
         <v>24</v>
       </c>
       <c r="R7" s="4">
-        <v>2.2000000000000002E-2</v>
+        <v>0.022000000000000002</v>
       </c>
       <c r="S7" s="4">
-        <v>5.4000000000000006E-2</v>
+        <v>0.054000000000000006</v>
       </c>
       <c r="T7" s="4">
         <v>2</v>
@@ -2483,7 +2482,7 @@
         <v>0.5</v>
       </c>
       <c r="AC7" s="4">
-        <v>2.4E-2</v>
+        <v>0.024</v>
       </c>
       <c r="AD7" s="4">
         <v>0.16</v>
@@ -2528,13 +2527,13 @@
         <v>2</v>
       </c>
       <c r="AR7" s="4">
-        <v>4.2000000000000003E-2</v>
+        <v>0.042</v>
       </c>
       <c r="AS7" s="4">
-        <v>2.2000000000000002E-2</v>
+        <v>0.022000000000000002</v>
       </c>
       <c r="AT7" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AU7" s="4">
         <v>6</v>
@@ -2543,10 +2542,10 @@
         <v>6</v>
       </c>
       <c r="AW7" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="AX7" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AY7" s="4">
         <v>6</v>
@@ -2555,10 +2554,10 @@
         <v>6</v>
       </c>
       <c r="BA7" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="BB7" s="4">
-        <v>4.0000000000000001E-3</v>
+        <v>0.004</v>
       </c>
       <c r="BC7" s="4">
         <v>1</v>
@@ -2573,7 +2572,7 @@
         <v>1.25</v>
       </c>
     </row>
-    <row r="8" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:58">
       <c r="B8" s="4">
         <v>5</v>
       </c>
@@ -2602,7 +2601,7 @@
         <v>2035</v>
       </c>
       <c r="K8" s="4">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="L8" s="4">
         <v>18</v>
@@ -2611,10 +2610,10 @@
         <v>18</v>
       </c>
       <c r="N8" s="4">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="O8" s="4">
-        <v>3.1E-2</v>
+        <v>0.031</v>
       </c>
       <c r="P8" s="4">
         <v>30</v>
@@ -2623,10 +2622,10 @@
         <v>24</v>
       </c>
       <c r="R8" s="4">
-        <v>1.95E-2</v>
+        <v>0.0195</v>
       </c>
       <c r="S8" s="4">
-        <v>5.4000000000000006E-2</v>
+        <v>0.054000000000000006</v>
       </c>
       <c r="T8" s="4">
         <v>5</v>
@@ -2653,7 +2652,7 @@
         <v>0.5</v>
       </c>
       <c r="AC8" s="4">
-        <v>2.4E-2</v>
+        <v>0.024</v>
       </c>
       <c r="AD8" s="4">
         <v>0.11</v>
@@ -2698,13 +2697,13 @@
         <v>1.5</v>
       </c>
       <c r="AR8" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="AS8" s="4">
-        <v>1.6E-2</v>
+        <v>0.016</v>
       </c>
       <c r="AT8" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AU8" s="4">
         <v>6</v>
@@ -2713,10 +2712,10 @@
         <v>6</v>
       </c>
       <c r="AW8" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="AX8" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AY8" s="4">
         <v>6</v>
@@ -2725,10 +2724,10 @@
         <v>6</v>
       </c>
       <c r="BA8" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="BB8" s="4">
-        <v>6.5000000000000006E-3</v>
+        <v>0.006500000000000001</v>
       </c>
       <c r="BC8" s="4">
         <v>3</v>
@@ -2743,7 +2742,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:58">
       <c r="B9" s="4">
         <v>11</v>
       </c>
@@ -2772,7 +2771,7 @@
         <v>2035</v>
       </c>
       <c r="K9" s="4">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="L9" s="4">
         <v>18</v>
@@ -2781,10 +2780,10 @@
         <v>18</v>
       </c>
       <c r="N9" s="4">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="O9" s="4">
-        <v>3.4000000000000002E-2</v>
+        <v>0.034</v>
       </c>
       <c r="P9" s="4">
         <v>30</v>
@@ -2793,10 +2792,10 @@
         <v>24</v>
       </c>
       <c r="R9" s="4">
-        <v>2.1499999999999998E-2</v>
+        <v>0.0215</v>
       </c>
       <c r="S9" s="4">
-        <v>4.9000000000000002E-2</v>
+        <v>0.049</v>
       </c>
       <c r="T9" s="4">
         <v>3.3</v>
@@ -2823,10 +2822,10 @@
         <v>0.5</v>
       </c>
       <c r="AC9" s="4">
-        <v>2.6000000000000002E-2</v>
+        <v>0.026000000000000002</v>
       </c>
       <c r="AD9" s="4">
-        <v>6.5000000000000002E-2</v>
+        <v>0.065</v>
       </c>
       <c r="AE9" s="4">
         <v>1</v>
@@ -2868,13 +2867,13 @@
         <v>1.5</v>
       </c>
       <c r="AR9" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="AS9" s="4">
-        <v>8.0000000000000002E-3</v>
+        <v>0.008</v>
       </c>
       <c r="AT9" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AU9" s="4">
         <v>6</v>
@@ -2883,10 +2882,10 @@
         <v>0</v>
       </c>
       <c r="AW9" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="AX9" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AY9" s="4">
         <v>6</v>
@@ -2895,10 +2894,10 @@
         <v>0</v>
       </c>
       <c r="BA9" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="BB9" s="4">
-        <v>4.0000000000000001E-3</v>
+        <v>0.004</v>
       </c>
       <c r="BC9" s="4">
         <v>6</v>
@@ -2913,7 +2912,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="10" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:58">
       <c r="B10" s="4">
         <v>2</v>
       </c>
@@ -2942,7 +2941,7 @@
         <v>2040</v>
       </c>
       <c r="K10" s="4">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="L10" s="4">
         <v>18</v>
@@ -2951,10 +2950,10 @@
         <v>18</v>
       </c>
       <c r="N10" s="4">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="O10" s="4">
-        <v>1.9E-2</v>
+        <v>0.016</v>
       </c>
       <c r="P10" s="4">
         <v>24</v>
@@ -2963,13 +2962,13 @@
         <v>36</v>
       </c>
       <c r="R10" s="4">
-        <v>1.3000000000000001E-2</v>
+        <v>0.013000000000000001</v>
       </c>
       <c r="S10" s="4">
-        <v>8.2500000000000004E-2</v>
+        <v>0.0825</v>
       </c>
       <c r="T10" s="4">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="V10" s="4">
         <v>15</v>
@@ -2981,10 +2980,10 @@
         <v>0</v>
       </c>
       <c r="Y10" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Z10" s="4">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="AA10" s="4">
         <v>0.15</v>
@@ -2999,10 +2998,10 @@
         <v>0.06</v>
       </c>
       <c r="AE10" s="4">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="AF10" s="4">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="AG10" s="4">
         <v>1</v>
@@ -3014,10 +3013,10 @@
         <v>0</v>
       </c>
       <c r="AJ10" s="4">
-        <v>1.2E-2</v>
+        <v>0.013999999999999999</v>
       </c>
       <c r="AK10" s="4">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="AL10" s="4">
         <v>180</v>
@@ -3029,22 +3028,22 @@
         <v>0.75</v>
       </c>
       <c r="AO10" s="4">
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="AP10" s="4">
-        <v>1.2</v>
+        <v>1.5</v>
       </c>
       <c r="AQ10" s="4">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AR10" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="AS10" s="4">
-        <v>7.4999999999999997E-3</v>
+        <v>0.0075</v>
       </c>
       <c r="AT10" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.012</v>
       </c>
       <c r="AU10" s="4">
         <v>6</v>
@@ -3053,10 +3052,10 @@
         <v>6</v>
       </c>
       <c r="AW10" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="AX10" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.012</v>
       </c>
       <c r="AY10" s="4">
         <v>6</v>
@@ -3065,10 +3064,10 @@
         <v>6</v>
       </c>
       <c r="BA10" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="BB10" s="4">
-        <v>1E-3</v>
+        <v>0.0005</v>
       </c>
       <c r="BC10" s="4">
         <v>0</v>
@@ -3083,7 +3082,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="11" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:58">
       <c r="B11" s="4">
         <v>7</v>
       </c>
@@ -3112,7 +3111,7 @@
         <v>2035</v>
       </c>
       <c r="K11" s="4">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="L11" s="4">
         <v>18</v>
@@ -3121,10 +3120,10 @@
         <v>18</v>
       </c>
       <c r="N11" s="4">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="O11" s="4">
-        <v>2.8500000000000001E-2</v>
+        <v>0.0285</v>
       </c>
       <c r="P11" s="4">
         <v>36</v>
@@ -3133,10 +3132,10 @@
         <v>24</v>
       </c>
       <c r="R11" s="4">
-        <v>2.1000000000000001E-2</v>
+        <v>0.021</v>
       </c>
       <c r="S11" s="4">
-        <v>7.2000000000000008E-2</v>
+        <v>0.07200000000000001</v>
       </c>
       <c r="T11" s="4">
         <v>4</v>
@@ -3184,7 +3183,7 @@
         <v>0</v>
       </c>
       <c r="AJ11" s="4">
-        <v>2.6000000000000002E-2</v>
+        <v>0.025</v>
       </c>
       <c r="AK11" s="4">
         <v>10</v>
@@ -3199,7 +3198,7 @@
         <v>0.65</v>
       </c>
       <c r="AO11" s="4">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="AP11" s="4">
         <v>2.5</v>
@@ -3208,13 +3207,13 @@
         <v>2</v>
       </c>
       <c r="AR11" s="4">
-        <v>5.2000000000000005E-2</v>
+        <v>0.052000000000000005</v>
       </c>
       <c r="AS11" s="4">
-        <v>1.6E-2</v>
+        <v>0.016</v>
       </c>
       <c r="AT11" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AU11" s="4">
         <v>6</v>
@@ -3223,10 +3222,10 @@
         <v>6</v>
       </c>
       <c r="AW11" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="AX11" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AY11" s="4">
         <v>6</v>
@@ -3235,10 +3234,10 @@
         <v>6</v>
       </c>
       <c r="BA11" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="BB11" s="4">
-        <v>1E-3</v>
+        <v>0.0005</v>
       </c>
       <c r="BC11" s="4">
         <v>4</v>
@@ -3250,10 +3249,10 @@
         <v>131</v>
       </c>
       <c r="BF11" s="4">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:58" x14ac:dyDescent="0.25">
+        <v>1.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:58">
       <c r="B12" s="4">
         <v>8</v>
       </c>
@@ -3282,7 +3281,7 @@
         <v>2035</v>
       </c>
       <c r="K12" s="4">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="L12" s="4">
         <v>18</v>
@@ -3291,10 +3290,10 @@
         <v>18</v>
       </c>
       <c r="N12" s="4">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="O12" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="P12" s="4">
         <v>36</v>
@@ -3303,10 +3302,10 @@
         <v>24</v>
       </c>
       <c r="R12" s="4">
-        <v>2.1000000000000001E-2</v>
+        <v>0.021</v>
       </c>
       <c r="S12" s="4">
-        <v>7.4800000000000005E-2</v>
+        <v>0.0748</v>
       </c>
       <c r="T12" s="4">
         <v>5</v>
@@ -3354,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="AJ12" s="4">
-        <v>1.8000000000000002E-2</v>
+        <v>0.018000000000000002</v>
       </c>
       <c r="AK12" s="4">
         <v>12</v>
@@ -3369,7 +3368,7 @@
         <v>0.65</v>
       </c>
       <c r="AO12" s="4">
-        <v>0.55000000000000004</v>
+        <v>0.55</v>
       </c>
       <c r="AP12" s="4">
         <v>1.25</v>
@@ -3378,13 +3377,13 @@
         <v>1.5</v>
       </c>
       <c r="AR12" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="AS12" s="4">
-        <v>1.2500000000000001E-2</v>
+        <v>0.0125</v>
       </c>
       <c r="AT12" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AU12" s="4">
         <v>6</v>
@@ -3393,10 +3392,10 @@
         <v>6</v>
       </c>
       <c r="AW12" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="AX12" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AY12" s="4">
         <v>6</v>
@@ -3405,10 +3404,10 @@
         <v>6</v>
       </c>
       <c r="BA12" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="BB12" s="4">
-        <v>1E-3</v>
+        <v>0.0005</v>
       </c>
       <c r="BC12" s="4">
         <v>4</v>
@@ -3423,7 +3422,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="13" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:58">
       <c r="B13" s="4">
         <v>9</v>
       </c>
@@ -3452,7 +3451,7 @@
         <v>2035</v>
       </c>
       <c r="K13" s="4">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="L13" s="4">
         <v>18</v>
@@ -3461,10 +3460,10 @@
         <v>18</v>
       </c>
       <c r="N13" s="4">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="O13" s="4">
-        <v>3.6000000000000004E-2</v>
+        <v>0.016</v>
       </c>
       <c r="P13" s="4">
         <v>36</v>
@@ -3473,10 +3472,10 @@
         <v>24</v>
       </c>
       <c r="R13" s="4">
-        <v>2.2000000000000002E-2</v>
+        <v>0.013000000000000001</v>
       </c>
       <c r="S13" s="4">
-        <v>8.8000000000000009E-2</v>
+        <v>0.06849999999999999</v>
       </c>
       <c r="T13" s="4">
         <v>5</v>
@@ -3491,7 +3490,7 @@
         <v>0</v>
       </c>
       <c r="Y13" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="Z13" s="4">
         <v>39</v>
@@ -3524,10 +3523,10 @@
         <v>0</v>
       </c>
       <c r="AJ13" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.0125</v>
       </c>
       <c r="AK13" s="4">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="AL13" s="4">
         <v>180</v>
@@ -3539,22 +3538,22 @@
         <v>0.65</v>
       </c>
       <c r="AO13" s="4">
-        <v>0.55000000000000004</v>
+        <v>0.35</v>
       </c>
       <c r="AP13" s="4">
         <v>1.25</v>
       </c>
       <c r="AQ13" s="4">
-        <v>1.5</v>
+        <v>2.5</v>
       </c>
       <c r="AR13" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="AS13" s="4">
-        <v>1.2500000000000001E-2</v>
+        <v>0.0125</v>
       </c>
       <c r="AT13" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AU13" s="4">
         <v>6</v>
@@ -3563,10 +3562,10 @@
         <v>6</v>
       </c>
       <c r="AW13" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="AX13" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AY13" s="4">
         <v>6</v>
@@ -3575,16 +3574,16 @@
         <v>6</v>
       </c>
       <c r="BA13" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="BB13" s="4">
-        <v>1E-3</v>
+        <v>0.0005</v>
       </c>
       <c r="BC13" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="BD13" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE13" s="4" t="s">
         <v>131</v>
@@ -3593,7 +3592,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="14" spans="1:58" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:58">
       <c r="B14" s="4">
         <v>10</v>
       </c>
@@ -3622,7 +3621,7 @@
         <v>2035</v>
       </c>
       <c r="K14" s="4">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="L14" s="4">
         <v>18</v>
@@ -3631,10 +3630,10 @@
         <v>18</v>
       </c>
       <c r="N14" s="4">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="O14" s="4">
-        <v>3.6000000000000004E-2</v>
+        <v>0.018000000000000002</v>
       </c>
       <c r="P14" s="4">
         <v>36</v>
@@ -3643,13 +3642,13 @@
         <v>24</v>
       </c>
       <c r="R14" s="4">
-        <v>2.2000000000000002E-2</v>
+        <v>0.015</v>
       </c>
       <c r="S14" s="4">
-        <v>7.4999999999999997E-2</v>
+        <v>0.0655</v>
       </c>
       <c r="T14" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="V14" s="4">
         <v>15</v>
@@ -3694,7 +3693,7 @@
         <v>0</v>
       </c>
       <c r="AJ14" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.022000000000000002</v>
       </c>
       <c r="AK14" s="4">
         <v>12</v>
@@ -3709,22 +3708,22 @@
         <v>0.65</v>
       </c>
       <c r="AO14" s="4">
-        <v>0.55000000000000004</v>
+        <v>0.45</v>
       </c>
       <c r="AP14" s="4">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="AQ14" s="4">
         <v>1.5</v>
       </c>
       <c r="AR14" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="AS14" s="4">
-        <v>1.2500000000000001E-2</v>
+        <v>0.0125</v>
       </c>
       <c r="AT14" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AU14" s="4">
         <v>6</v>
@@ -3733,10 +3732,10 @@
         <v>6</v>
       </c>
       <c r="AW14" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="AX14" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AY14" s="4">
         <v>6</v>
@@ -3745,10 +3744,10 @@
         <v>6</v>
       </c>
       <c r="BA14" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="BB14" s="4">
-        <v>1E-3</v>
+        <v>0.0005</v>
       </c>
       <c r="BC14" s="4">
         <v>6</v>
@@ -3764,7 +3763,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
@@ -3774,36 +3773,36 @@
   <sheetViews>
     <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="45.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="45.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="45.85546875" style="1"/>
+    <col bestFit="true" customWidth="true" max="1" min="1" style="1" width="2"/>
+    <col bestFit="true" customWidth="true" max="2" min="2" style="1" width="9"/>
+    <col customWidth="true" max="3" min="3" style="1" width="11.28515625"/>
+    <col bestFit="true" customWidth="true" max="4" min="4" style="1" width="17"/>
+    <col bestFit="true" customWidth="true" max="5" min="5" style="1" width="18.28515625"/>
+    <col bestFit="true" customWidth="true" max="6" min="6" style="1" width="16.140625"/>
+    <col bestFit="true" customWidth="true" max="7" min="7" style="1" width="17.42578125"/>
+    <col bestFit="true" customWidth="true" max="8" min="8" style="1" width="15.28515625"/>
+    <col bestFit="true" customWidth="true" max="9" min="9" style="1" width="11"/>
+    <col bestFit="true" customWidth="true" max="10" min="10" style="1" width="20.28515625"/>
+    <col bestFit="true" customWidth="true" max="11" min="11" style="1" width="12.7109375"/>
+    <col bestFit="true" customWidth="true" max="12" min="12" style="1" width="10.7109375"/>
+    <col bestFit="true" customWidth="true" max="13" min="13" style="1" width="18.42578125"/>
+    <col bestFit="true" customWidth="true" max="14" min="14" style="1" width="12.85546875"/>
+    <col bestFit="true" customWidth="true" max="15" min="15" style="1" width="10.7109375"/>
+    <col bestFit="true" customWidth="true" max="16" min="16" style="1" width="11.28515625"/>
+    <col bestFit="true" customWidth="true" max="17" min="17" style="1" width="18.28515625"/>
+    <col bestFit="true" customWidth="true" max="18" min="18" style="1" width="18.140625"/>
+    <col bestFit="true" customWidth="true" max="19" min="19" style="1" width="18.28515625"/>
+    <col bestFit="true" customWidth="true" max="20" min="20" style="1" width="5.140625"/>
+    <col bestFit="true" customWidth="true" max="21" min="21" style="1" width="13.42578125"/>
+    <col bestFit="true" customWidth="true" max="22" min="22" style="1" width="8.5703125"/>
+    <col bestFit="true" customWidth="true" max="23" min="23" style="1" width="11.5703125"/>
+    <col bestFit="true" customWidth="true" max="24" min="24" style="1" width="17.5703125"/>
+    <col max="16384" min="25" style="1" width="45.85546875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -3877,7 +3876,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3948,7 +3947,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -3987,7 +3986,7 @@
       </c>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -4026,7 +4025,7 @@
       </c>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -4065,7 +4064,7 @@
       </c>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -4104,7 +4103,7 @@
       </c>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -4143,7 +4142,7 @@
       </c>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -4182,7 +4181,7 @@
       </c>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -4221,7 +4220,7 @@
       </c>
       <c r="X9" s="2"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -4260,7 +4259,7 @@
       </c>
       <c r="X10" s="2"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -4298,7 +4297,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -4336,7 +4335,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -4375,7 +4374,7 @@
       </c>
       <c r="X13" s="2"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -4413,7 +4412,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -4451,7 +4450,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -4489,7 +4488,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:23">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -4527,7 +4526,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:23">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -4565,7 +4564,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:23">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -4603,7 +4602,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:23">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -4641,7 +4640,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:23">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -4679,7 +4678,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:23">
       <c r="B22" s="1">
         <v>20</v>
       </c>
@@ -4717,7 +4716,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:23">
       <c r="B23" s="1">
         <v>21</v>
       </c>
@@ -4755,7 +4754,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:23">
       <c r="B24" s="1">
         <v>22</v>
       </c>
@@ -4793,7 +4792,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:23">
       <c r="B25" s="1">
         <v>23</v>
       </c>
@@ -4831,7 +4830,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:23">
       <c r="B26" s="1">
         <v>24</v>
       </c>
@@ -4869,7 +4868,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:23">
       <c r="B27" s="1">
         <v>25</v>
       </c>
@@ -4907,7 +4906,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:23">
       <c r="B28" s="1">
         <v>26</v>
       </c>
@@ -4945,7 +4944,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:23">
       <c r="B29" s="1">
         <v>27</v>
       </c>
@@ -4983,7 +4982,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:23">
       <c r="B30" s="1">
         <v>28</v>
       </c>
@@ -5021,7 +5020,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:23">
       <c r="B31" s="1">
         <v>29</v>
       </c>
@@ -5059,7 +5058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:23">
       <c r="B32" s="1">
         <v>30</v>
       </c>
@@ -5097,7 +5096,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:23">
       <c r="B33" s="1">
         <v>31</v>
       </c>
@@ -5135,9 +5134,47 @@
         <v>15</v>
       </c>
     </row>
+    <row r="34">
+      <c r="B34" s="1">
+        <v>32</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D34" s="1">
+        <v>9</v>
+      </c>
+      <c r="E34" s="1">
+        <v>1</v>
+      </c>
+      <c r="F34" s="1">
+        <v>2017</v>
+      </c>
+      <c r="G34" s="1">
+        <v>12</v>
+      </c>
+      <c r="H34" s="1">
+        <v>2050</v>
+      </c>
+      <c r="I34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="K34" s="1">
+        <v>4500000</v>
+      </c>
+      <c r="V34" s="1">
+        <v>250000</v>
+      </c>
+      <c r="W34" s="1">
+        <v>18</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Azure parallelism & metrics table
</commit_message>
<xml_diff>
--- a/models/Data.xlsx
+++ b/models/Data.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView windowHeight="23500" windowWidth="38620" xWindow="-38510" yWindow="-110"/>
+    <workbookView windowHeight="31920" windowWidth="57840" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -1333,8 +1333,8 @@
   <dimension ref="A1:BG14"/>
   <sheetViews>
     <sheetView tabSelected="true" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane activePane="topRight" state="frozen" topLeftCell="AY1" xSplit="3"/>
-      <selection activeCell="BG4" pane="topRight" sqref="BG4:BG14"/>
+      <pane activePane="topRight" state="frozen" topLeftCell="D1" xSplit="3"/>
+      <selection activeCell="AR6" pane="topRight" sqref="AR6:AR9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15"/>
@@ -1918,7 +1918,7 @@
         <v>1.6</v>
       </c>
       <c r="BG3" s="6">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:59">
@@ -2085,7 +2085,7 @@
         <v>0</v>
       </c>
       <c r="BG4" s="6">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:59">
@@ -2250,7 +2250,7 @@
         <v>0</v>
       </c>
       <c r="BG5" s="6">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:59">
@@ -2372,40 +2372,40 @@
         <v>0</v>
       </c>
       <c r="AP6" s="4">
-        <v>1.45</v>
+        <v>0</v>
       </c>
       <c r="AQ6" s="4">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="AR6" s="4">
-        <v>0.032</v>
+        <v>0.025</v>
       </c>
       <c r="AS6" s="4">
-        <v>0.022000000000000002</v>
+        <v>0.03</v>
       </c>
       <c r="AT6" s="4">
-        <v>0.006999999999999999</v>
+        <v>0</v>
       </c>
       <c r="AU6" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AV6" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AW6" s="4">
-        <v>0.0015</v>
+        <v>0</v>
       </c>
       <c r="AX6" s="4">
-        <v>0.006999999999999999</v>
+        <v>0</v>
       </c>
       <c r="AY6" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="AZ6" s="4">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="BA6" s="4">
-        <v>0.0015</v>
+        <v>0</v>
       </c>
       <c r="BB6" s="4">
         <v>0.0005</v>
@@ -2423,7 +2423,7 @@
         <v>14</v>
       </c>
       <c r="BG6" s="6">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="7" spans="1:59">
@@ -2455,7 +2455,7 @@
         <v>2035</v>
       </c>
       <c r="K7" s="4">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="L7" s="4">
         <v>18</v>
@@ -2464,10 +2464,10 @@
         <v>18</v>
       </c>
       <c r="N7" s="4">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="O7" s="4">
-        <v>2.8500000000000001E-2</v>
+        <v>0.0285</v>
       </c>
       <c r="P7" s="4">
         <v>36</v>
@@ -2476,10 +2476,10 @@
         <v>24</v>
       </c>
       <c r="R7" s="4">
-        <v>2.2000000000000002E-2</v>
+        <v>0.022000000000000002</v>
       </c>
       <c r="S7" s="4">
-        <v>5.4000000000000006E-2</v>
+        <v>0.054000000000000006</v>
       </c>
       <c r="T7" s="4">
         <v>2</v>
@@ -2506,7 +2506,7 @@
         <v>0.5</v>
       </c>
       <c r="AC7" s="4">
-        <v>2.4E-2</v>
+        <v>0.024</v>
       </c>
       <c r="AD7" s="4">
         <v>0.16</v>
@@ -2545,43 +2545,43 @@
         <v>0</v>
       </c>
       <c r="AP7" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AQ7" s="4">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="AR7" s="4">
-        <v>0</v>
+        <v>0.027000000000000003</v>
       </c>
       <c r="AS7" s="4">
         <v>0</v>
       </c>
       <c r="AT7" s="4">
-        <v>0</v>
+        <v>0.008</v>
       </c>
       <c r="AU7" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AV7" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AW7" s="4">
-        <v>0</v>
+        <v>0.0015</v>
       </c>
       <c r="AX7" s="4">
-        <v>0</v>
+        <v>0.008</v>
       </c>
       <c r="AY7" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AZ7" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BA7" s="4">
-        <v>0</v>
+        <v>0.0015</v>
       </c>
       <c r="BB7" s="4">
-        <v>4.0000000000000001E-3</v>
+        <v>0.004</v>
       </c>
       <c r="BC7" s="4">
         <v>1</v>
@@ -2628,7 +2628,7 @@
         <v>2035</v>
       </c>
       <c r="K8" s="4">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="L8" s="4">
         <v>18</v>
@@ -2637,10 +2637,10 @@
         <v>18</v>
       </c>
       <c r="N8" s="4">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="O8" s="4">
-        <v>3.1E-2</v>
+        <v>0.031</v>
       </c>
       <c r="P8" s="4">
         <v>30</v>
@@ -2649,13 +2649,13 @@
         <v>24</v>
       </c>
       <c r="R8" s="4">
-        <v>1.95E-2</v>
+        <v>0.0195</v>
       </c>
       <c r="S8" s="4">
-        <v>5.4000000000000006E-2</v>
+        <v>0.054000000000000006</v>
       </c>
       <c r="T8" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="V8" s="4">
         <v>10</v>
@@ -2679,7 +2679,7 @@
         <v>0.5</v>
       </c>
       <c r="AC8" s="4">
-        <v>2.4E-2</v>
+        <v>0.024</v>
       </c>
       <c r="AD8" s="4">
         <v>0.11</v>
@@ -2709,52 +2709,52 @@
         <v>60</v>
       </c>
       <c r="AM8" s="4">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="AN8" s="4">
-        <v>0.65</v>
+        <v>0.75</v>
       </c>
       <c r="AO8" s="4">
         <v>0</v>
       </c>
       <c r="AP8" s="4">
-        <v>0</v>
+        <v>0.75</v>
       </c>
       <c r="AQ8" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AR8" s="4">
-        <v>0</v>
+        <v>0.025</v>
       </c>
       <c r="AS8" s="4">
-        <v>0</v>
+        <v>0.013999999999999999</v>
       </c>
       <c r="AT8" s="4">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="AU8" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AV8" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AW8" s="4">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="AX8" s="4">
-        <v>0</v>
+        <v>0.004</v>
       </c>
       <c r="AY8" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AZ8" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BA8" s="4">
-        <v>0</v>
+        <v>0.001</v>
       </c>
       <c r="BB8" s="4">
-        <v>6.5000000000000006E-3</v>
+        <v>0.001</v>
       </c>
       <c r="BC8" s="4">
         <v>3</v>
@@ -2801,7 +2801,7 @@
         <v>2035</v>
       </c>
       <c r="K9" s="4">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="L9" s="4">
         <v>18</v>
@@ -2810,22 +2810,22 @@
         <v>18</v>
       </c>
       <c r="N9" s="4">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="O9" s="4">
-        <v>3.4000000000000002E-2</v>
+        <v>0.034</v>
       </c>
       <c r="P9" s="4">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="Q9" s="4">
         <v>24</v>
       </c>
       <c r="R9" s="4">
-        <v>2.1499999999999998E-2</v>
+        <v>0.0215</v>
       </c>
       <c r="S9" s="4">
-        <v>4.9000000000000002E-2</v>
+        <v>0.049</v>
       </c>
       <c r="T9" s="4">
         <v>3.3</v>
@@ -2852,10 +2852,10 @@
         <v>0.5</v>
       </c>
       <c r="AC9" s="4">
-        <v>2.6000000000000002E-2</v>
+        <v>0.026000000000000002</v>
       </c>
       <c r="AD9" s="4">
-        <v>6.5000000000000002E-2</v>
+        <v>0.065</v>
       </c>
       <c r="AE9" s="4">
         <v>1</v>
@@ -2885,49 +2885,49 @@
         <v>1</v>
       </c>
       <c r="AN9" s="4">
-        <v>0.65</v>
+        <v>0.75</v>
       </c>
       <c r="AO9" s="4">
         <v>0</v>
       </c>
       <c r="AP9" s="4">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="AQ9" s="4">
-        <v>0</v>
+        <v>1.6</v>
       </c>
       <c r="AR9" s="4">
-        <v>0</v>
+        <v>0.027000000000000003</v>
       </c>
       <c r="AS9" s="4">
-        <v>0</v>
+        <v>0.008</v>
       </c>
       <c r="AT9" s="4">
-        <v>0</v>
+        <v>0.008</v>
       </c>
       <c r="AU9" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AV9" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AW9" s="4">
-        <v>0</v>
+        <v>0.0015</v>
       </c>
       <c r="AX9" s="4">
-        <v>0</v>
+        <v>0.008</v>
       </c>
       <c r="AY9" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AZ9" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="BA9" s="4">
-        <v>0</v>
+        <v>0.0015</v>
       </c>
       <c r="BB9" s="4">
-        <v>4.0000000000000001E-3</v>
+        <v>0.0005</v>
       </c>
       <c r="BC9" s="4">
         <v>6</v>
@@ -2942,7 +2942,7 @@
         <v>2.9</v>
       </c>
       <c r="BG9" s="6">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="10" spans="1:59">
@@ -2974,37 +2974,37 @@
         <v>2040</v>
       </c>
       <c r="K10" s="4">
-        <v>0.055</v>
+        <v>0.05</v>
       </c>
       <c r="L10" s="4">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="M10" s="4">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="N10" s="4">
-        <v>0.019</v>
+        <v>0.013999999999999999</v>
       </c>
       <c r="O10" s="4">
-        <v>0.016</v>
+        <v>0</v>
       </c>
       <c r="P10" s="4">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="Q10" s="4">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="R10" s="4">
-        <v>0.013000000000000001</v>
+        <v>0.012</v>
       </c>
       <c r="S10" s="4">
-        <v>0.0825</v>
+        <v>0.06</v>
       </c>
       <c r="T10" s="4">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="V10" s="4">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="W10" s="4">
         <v>0</v>
@@ -3028,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="AD10" s="4">
-        <v>0.06</v>
+        <v>0.1275</v>
       </c>
       <c r="AE10" s="4">
         <v>10</v>
@@ -3037,7 +3037,7 @@
         <v>10</v>
       </c>
       <c r="AG10" s="4">
-        <v>1</v>
+        <v>0.87</v>
       </c>
       <c r="AH10" s="4" t="s">
         <v>113</v>
@@ -3046,13 +3046,13 @@
         <v>0</v>
       </c>
       <c r="AJ10" s="4">
-        <v>0.018000000000000002</v>
+        <v>0.029900000000000003</v>
       </c>
       <c r="AK10" s="4">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="AL10" s="4">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="AM10" s="4">
         <v>1</v>
@@ -3061,10 +3061,10 @@
         <v>0.75</v>
       </c>
       <c r="AO10" s="4">
-        <v>0.34</v>
+        <v>0.6</v>
       </c>
       <c r="AP10" s="4">
-        <v>1.5</v>
+        <v>2</v>
       </c>
       <c r="AQ10" s="4">
         <v>1.6</v>
@@ -3079,10 +3079,10 @@
         <v>0.008</v>
       </c>
       <c r="AU10" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AV10" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AW10" s="4">
         <v>0.0015</v>
@@ -3091,10 +3091,10 @@
         <v>0.008</v>
       </c>
       <c r="AY10" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="AZ10" s="4">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="BA10" s="4">
         <v>0.0015</v>
@@ -3288,7 +3288,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="BG11" s="6">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:59">
@@ -3320,7 +3320,7 @@
         <v>2035</v>
       </c>
       <c r="K12" s="4">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="L12" s="4">
         <v>18</v>
@@ -3329,10 +3329,10 @@
         <v>18</v>
       </c>
       <c r="N12" s="4">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="O12" s="4">
-        <v>1.7000000000000001E-2</v>
+        <v>0.017</v>
       </c>
       <c r="P12" s="4">
         <v>36</v>
@@ -3341,16 +3341,16 @@
         <v>24</v>
       </c>
       <c r="R12" s="4">
-        <v>1.3999999999999999E-2</v>
+        <v>0.013999999999999999</v>
       </c>
       <c r="S12" s="4">
-        <v>7.4800000000000005E-2</v>
+        <v>0.05</v>
       </c>
       <c r="T12" s="4">
         <v>5</v>
       </c>
       <c r="V12" s="4">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="W12" s="4">
         <v>0</v>
@@ -3383,7 +3383,7 @@
         <v>6</v>
       </c>
       <c r="AG12" s="4">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="AH12" s="4" t="s">
         <v>113</v>
@@ -3392,7 +3392,7 @@
         <v>0</v>
       </c>
       <c r="AJ12" s="4">
-        <v>1.8500000000000003E-2</v>
+        <v>0.018500000000000003</v>
       </c>
       <c r="AK12" s="4">
         <v>12</v>
@@ -3407,7 +3407,7 @@
         <v>0.65</v>
       </c>
       <c r="AO12" s="4">
-        <v>0.45</v>
+        <v>0.6</v>
       </c>
       <c r="AP12" s="4">
         <v>1.25</v>
@@ -3416,13 +3416,13 @@
         <v>1.5</v>
       </c>
       <c r="AR12" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="AS12" s="4">
-        <v>1.2500000000000001E-2</v>
+        <v>0.0125</v>
       </c>
       <c r="AT12" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AU12" s="4">
         <v>6</v>
@@ -3431,10 +3431,10 @@
         <v>6</v>
       </c>
       <c r="AW12" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="AX12" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AY12" s="4">
         <v>6</v>
@@ -3443,10 +3443,10 @@
         <v>6</v>
       </c>
       <c r="BA12" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="BB12" s="4">
-        <v>5.0000000000000001E-4</v>
+        <v>0.0005</v>
       </c>
       <c r="BC12" s="4">
         <v>4</v>
@@ -3461,7 +3461,7 @@
         <v>0.8</v>
       </c>
       <c r="BG12" s="6">
-        <v>100</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:59">
@@ -3493,7 +3493,7 @@
         <v>2035</v>
       </c>
       <c r="K13" s="4">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="L13" s="4">
         <v>18</v>
@@ -3502,28 +3502,28 @@
         <v>18</v>
       </c>
       <c r="N13" s="4">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="O13" s="4">
-        <v>2.6499999999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="P13" s="4">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="Q13" s="4">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="R13" s="4">
-        <v>2.2000000000000002E-2</v>
+        <v>0.012</v>
       </c>
       <c r="S13" s="4">
-        <v>5.8499999999999996E-2</v>
+        <v>0.084</v>
       </c>
       <c r="T13" s="4">
         <v>2.5</v>
       </c>
       <c r="V13" s="4">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="W13" s="4">
         <v>0</v>
@@ -3547,7 +3547,7 @@
         <v>0</v>
       </c>
       <c r="AD13" s="4">
-        <v>0.09</v>
+        <v>0.15</v>
       </c>
       <c r="AE13" s="4">
         <v>1</v>
@@ -3556,7 +3556,7 @@
         <v>6</v>
       </c>
       <c r="AG13" s="4">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="AH13" s="4" t="s">
         <v>113</v>
@@ -3565,13 +3565,13 @@
         <v>0.4</v>
       </c>
       <c r="AJ13" s="4">
-        <v>1.4999999999999999E-2</v>
+        <v>0.0149</v>
       </c>
       <c r="AK13" s="4">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="AL13" s="4">
-        <v>180</v>
+        <v>240</v>
       </c>
       <c r="AM13" s="4">
         <v>1</v>
@@ -3580,22 +3580,22 @@
         <v>0.65</v>
       </c>
       <c r="AO13" s="4">
-        <v>0.5</v>
+        <v>0.45</v>
       </c>
       <c r="AP13" s="4">
-        <v>1.25</v>
+        <v>0.75</v>
       </c>
       <c r="AQ13" s="4">
         <v>1.5</v>
       </c>
       <c r="AR13" s="4">
-        <v>2.5000000000000001E-2</v>
+        <v>0.025</v>
       </c>
       <c r="AS13" s="4">
-        <v>1.2500000000000001E-2</v>
+        <v>0.0125</v>
       </c>
       <c r="AT13" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AU13" s="4">
         <v>6</v>
@@ -3604,10 +3604,10 @@
         <v>6</v>
       </c>
       <c r="AW13" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="AX13" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AY13" s="4">
         <v>6</v>
@@ -3616,16 +3616,16 @@
         <v>6</v>
       </c>
       <c r="BA13" s="4">
-        <v>2.5000000000000001E-3</v>
+        <v>0.0025</v>
       </c>
       <c r="BB13" s="4">
-        <v>5.0000000000000001E-4</v>
+        <v>0.0001</v>
       </c>
       <c r="BC13" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BD13" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE13" s="4" t="s">
         <v>131</v>
@@ -3634,7 +3634,7 @@
         <v>0.8</v>
       </c>
       <c r="BG13" s="6">
-        <v>100</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:59">
@@ -3666,7 +3666,7 @@
         <v>2035</v>
       </c>
       <c r="K14" s="4">
-        <v>5.5E-2</v>
+        <v>0.055</v>
       </c>
       <c r="L14" s="4">
         <v>18</v>
@@ -3675,10 +3675,10 @@
         <v>18</v>
       </c>
       <c r="N14" s="4">
-        <v>1.9E-2</v>
+        <v>0.019</v>
       </c>
       <c r="O14" s="4">
-        <v>2.1000000000000001E-2</v>
+        <v>0.021</v>
       </c>
       <c r="P14" s="4">
         <v>36</v>
@@ -3687,7 +3687,7 @@
         <v>24</v>
       </c>
       <c r="R14" s="4">
-        <v>1.7500000000000002E-2</v>
+        <v>0.0175</v>
       </c>
       <c r="S14" s="4">
         <v>0.06</v>
@@ -3738,7 +3738,7 @@
         <v>0.4</v>
       </c>
       <c r="AJ14" s="4">
-        <v>1.4999999999999999E-2</v>
+        <v>0.015</v>
       </c>
       <c r="AK14" s="4">
         <v>9</v>
@@ -3762,13 +3762,13 @@
         <v>1.5</v>
       </c>
       <c r="AR14" s="4">
-        <v>3.5000000000000003E-2</v>
+        <v>0.035</v>
       </c>
       <c r="AS14" s="4">
-        <v>1.2500000000000001E-2</v>
+        <v>0.0125</v>
       </c>
       <c r="AT14" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AU14" s="4">
         <v>6</v>
@@ -3777,10 +3777,10 @@
         <v>6</v>
       </c>
       <c r="AW14" s="4">
-        <v>1.5E-3</v>
+        <v>0.0015</v>
       </c>
       <c r="AX14" s="4">
-        <v>6.9999999999999993E-3</v>
+        <v>0.006999999999999999</v>
       </c>
       <c r="AY14" s="4">
         <v>6</v>
@@ -3789,10 +3789,10 @@
         <v>6</v>
       </c>
       <c r="BA14" s="4">
-        <v>1.5E-3</v>
+        <v>0.0015</v>
       </c>
       <c r="BB14" s="4">
-        <v>5.0000000000000001E-4</v>
+        <v>0.0005</v>
       </c>
       <c r="BC14" s="4">
         <v>3</v>

</xml_diff>

<commit_message>
SQLite, updated entities & calcs. NO MONTE CARLO
</commit_message>
<xml_diff>
--- a/models/Data.xlsx
+++ b/models/Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <bookViews>
-    <workbookView windowHeight="31920" windowWidth="57840" xWindow="-120" yWindow="-120"/>
+    <workbookView windowHeight="23500" windowWidth="38620" xWindow="-110" yWindow="-110"/>
   </bookViews>
   <sheets>
-    <sheet name="Entities" sheetId="1" r:id="rId1"/>
-    <sheet name="Units" sheetId="2" r:id="rId2"/>
-    <sheet name="Growth Items(OLD)" sheetId="4" r:id="rId3"/>
+    <sheet name="Entities" sheetId="5" r:id="rId1"/>
+    <sheet name="EntityModels" sheetId="1" r:id="rId2"/>
+    <sheet name="UnitModels" sheetId="2" r:id="rId3"/>
+    <sheet name="Growth Items(OLD)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="156">
   <si>
     <t>RETT</t>
   </si>
@@ -459,6 +460,42 @@
   </si>
   <si>
     <t>Sims</t>
+  </si>
+  <si>
+    <t>ParentID</t>
+  </si>
+  <si>
+    <t>EntityType</t>
+  </si>
+  <si>
+    <t>Entity</t>
+  </si>
+  <si>
+    <t>Fund</t>
+  </si>
+  <si>
+    <t>Asset</t>
+  </si>
+  <si>
+    <t>Acq Month</t>
+  </si>
+  <si>
+    <t>Acq Year</t>
+  </si>
+  <si>
+    <t>Disp Month</t>
+  </si>
+  <si>
+    <t>Disp Year</t>
+  </si>
+  <si>
+    <t>blank</t>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>v1</t>
   </si>
 </sst>
 </file>
@@ -954,7 +991,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="true">
       <alignment wrapText="true"/>
@@ -973,6 +1010,9 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="true" applyFont="true" applyAlignment="true">
       <alignment horizontal="center" vertical="center" wrapText="true"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="true" applyFont="true" applyAlignment="true">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1329,76 +1369,467 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12BAA125-4F8A-434B-82B0-238C2CAE36E0}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="184" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.08984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="8" width="14" customWidth="1"/>
+    <col min="9" max="9" width="9.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>144</v>
+      </c>
+      <c r="E2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G2" t="s">
+        <v>151</v>
+      </c>
+      <c r="H2" t="s">
+        <v>152</v>
+      </c>
+      <c r="I2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="s">
+        <v>153</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <v>2018</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <v>2016</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+      <c r="D6">
+        <v>3</v>
+      </c>
+      <c r="E6">
+        <v>7</v>
+      </c>
+      <c r="F6">
+        <v>2018</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>2018</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>134</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="F8">
+        <v>2019</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>135</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>10</v>
+      </c>
+      <c r="F9">
+        <v>2019</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10">
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <v>4</v>
+      </c>
+      <c r="F10">
+        <v>2016</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>7</v>
+      </c>
+      <c r="C11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D11">
+        <v>6</v>
+      </c>
+      <c r="E11">
+        <v>5</v>
+      </c>
+      <c r="F11">
+        <v>2016</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12">
+        <v>6</v>
+      </c>
+      <c r="E12">
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <v>2016</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>9</v>
+      </c>
+      <c r="C13" t="s">
+        <v>116</v>
+      </c>
+      <c r="D13">
+        <v>6</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="F13">
+        <v>2017</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14" t="s">
+        <v>117</v>
+      </c>
+      <c r="D14">
+        <v>6</v>
+      </c>
+      <c r="E14">
+        <v>5</v>
+      </c>
+      <c r="F14">
+        <v>2017</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BG14"/>
+  <dimension ref="A1:BI19"/>
   <sheetViews>
-    <sheetView tabSelected="true" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane activePane="topRight" state="frozen" topLeftCell="D1" xSplit="3"/>
-      <selection activeCell="AR6" pane="topRight" sqref="AR6:AR9"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane activePane="bottomRight" state="frozen" topLeftCell="D3" xSplit="3" ySplit="2"/>
+      <selection activeCell="D1" pane="topRight" sqref="D1"/>
+      <selection activeCell="A3" pane="bottomLeft" sqref="A3"/>
+      <selection activeCell="D7" pane="bottomRight" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="12.54296875" defaultRowHeight="14.5"/>
   <cols>
-    <col bestFit="true" customWidth="true" max="1" min="1" style="4" width="5.140625"/>
-    <col bestFit="true" customWidth="true" max="2" min="2" style="4" width="9.140625"/>
-    <col bestFit="true" customWidth="true" max="3" min="3" style="4" width="15.7109375"/>
-    <col bestFit="true" customWidth="true" max="4" min="4" style="4" width="8.42578125"/>
-    <col bestFit="true" customWidth="true" max="5" min="5" style="4" width="12.140625"/>
-    <col bestFit="true" customWidth="true" max="6" min="6" style="4" width="11.7109375"/>
-    <col customWidth="true" max="7" min="7" style="4" width="12.42578125"/>
-    <col bestFit="true" customWidth="true" max="8" min="8" style="4" width="11.7109375"/>
+    <col bestFit="true" customWidth="true" max="1" min="1" style="4" width="5.1796875"/>
+    <col bestFit="true" customWidth="true" max="2" min="2" style="4" width="9.1796875"/>
+    <col bestFit="true" customWidth="true" max="3" min="3" style="4" width="24.54296875"/>
+    <col bestFit="true" customWidth="true" max="4" min="4" style="4" width="8.6328125"/>
+    <col bestFit="true" customWidth="true" max="5" min="5" style="4" width="12.1796875"/>
+    <col bestFit="true" customWidth="true" max="6" min="6" style="4" width="11.7265625"/>
+    <col customWidth="true" max="7" min="7" style="4" width="12.453125"/>
+    <col bestFit="true" customWidth="true" max="8" min="8" style="4" width="11.7265625"/>
     <col bestFit="true" customWidth="true" max="9" min="9" style="4" width="10"/>
-    <col bestFit="true" customWidth="true" max="10" min="10" style="4" width="11.7109375"/>
-    <col bestFit="true" customWidth="true" max="11" min="11" style="4" width="18.28515625"/>
-    <col bestFit="true" customWidth="true" max="12" min="12" style="4" width="14.5703125"/>
-    <col bestFit="true" customWidth="true" max="13" min="13" style="4" width="18.7109375"/>
-    <col bestFit="true" customWidth="true" max="14" min="14" style="4" width="8.85546875"/>
-    <col bestFit="true" customWidth="true" max="15" min="15" style="4" width="17.7109375"/>
-    <col bestFit="true" customWidth="true" max="16" min="16" style="4" width="20.28515625"/>
-    <col bestFit="true" customWidth="true" max="17" min="17" style="4" width="13.28515625"/>
-    <col bestFit="true" customWidth="true" max="18" min="18" style="4" width="13.85546875"/>
-    <col bestFit="true" customWidth="true" max="19" min="19" style="4" width="10.5703125"/>
+    <col bestFit="true" customWidth="true" max="10" min="10" style="4" width="11.7265625"/>
+    <col bestFit="true" customWidth="true" max="11" min="11" style="4" width="18.26953125"/>
+    <col bestFit="true" customWidth="true" max="12" min="12" style="4" width="14.54296875"/>
+    <col bestFit="true" customWidth="true" max="13" min="13" style="4" width="18.7265625"/>
+    <col bestFit="true" customWidth="true" max="14" min="14" style="4" width="8.81640625"/>
+    <col bestFit="true" customWidth="true" max="15" min="15" style="4" width="17.7265625"/>
+    <col bestFit="true" customWidth="true" max="16" min="16" style="4" width="20.26953125"/>
+    <col bestFit="true" customWidth="true" max="17" min="17" style="4" width="13.26953125"/>
+    <col bestFit="true" customWidth="true" max="18" min="18" style="4" width="13.81640625"/>
+    <col bestFit="true" customWidth="true" max="19" min="19" style="4" width="10.54296875"/>
     <col bestFit="true" customWidth="true" max="20" min="20" style="4" width="11"/>
-    <col bestFit="true" customWidth="true" max="21" min="21" style="4" width="9.28515625"/>
-    <col bestFit="true" customWidth="true" max="22" min="22" style="4" width="11.42578125"/>
-    <col bestFit="true" customWidth="true" max="23" min="23" style="4" width="5.5703125"/>
-    <col bestFit="true" customWidth="true" max="24" min="24" style="4" width="5.140625"/>
-    <col bestFit="true" customWidth="true" max="25" min="25" style="4" width="13.7109375"/>
-    <col bestFit="true" customWidth="true" max="26" min="26" style="4" width="11.7109375"/>
+    <col bestFit="true" customWidth="true" max="21" min="21" style="4" width="9.26953125"/>
+    <col bestFit="true" customWidth="true" max="22" min="22" style="4" width="11.453125"/>
+    <col bestFit="true" customWidth="true" max="23" min="23" style="4" width="5.54296875"/>
+    <col bestFit="true" customWidth="true" max="24" min="24" style="4" width="5.1796875"/>
+    <col bestFit="true" customWidth="true" max="25" min="25" style="4" width="13.7265625"/>
+    <col bestFit="true" customWidth="true" max="26" min="26" style="4" width="11.7265625"/>
     <col bestFit="true" customWidth="true" max="27" min="27" style="4" width="11"/>
     <col bestFit="true" customWidth="true" max="28" min="28" style="4" width="8"/>
     <col bestFit="true" customWidth="true" max="29" min="29" style="4" width="10"/>
-    <col bestFit="true" customWidth="true" max="30" min="30" style="4" width="14.140625"/>
+    <col bestFit="true" customWidth="true" max="30" min="30" style="4" width="14.1796875"/>
     <col bestFit="true" customWidth="true" max="31" min="31" style="4" width="12"/>
-    <col bestFit="true" customWidth="true" max="32" min="32" style="4" width="14.5703125"/>
-    <col bestFit="true" customWidth="true" max="33" min="33" style="4" width="19.5703125"/>
-    <col bestFit="true" customWidth="true" max="34" min="34" style="4" width="10.28515625"/>
+    <col bestFit="true" customWidth="true" max="32" min="32" style="4" width="14.54296875"/>
+    <col bestFit="true" customWidth="true" max="33" min="33" style="4" width="19.54296875"/>
+    <col bestFit="true" customWidth="true" max="34" min="34" style="4" width="10.26953125"/>
     <col bestFit="true" customWidth="true" max="35" min="35" style="4" width="8"/>
-    <col bestFit="true" customWidth="true" max="36" min="36" style="4" width="12.42578125"/>
-    <col bestFit="true" customWidth="true" max="37" min="37" style="4" width="9.140625"/>
-    <col bestFit="true" customWidth="true" max="38" min="38" style="4" width="10.140625"/>
-    <col bestFit="true" customWidth="true" max="39" min="39" style="4" width="16.140625"/>
+    <col bestFit="true" customWidth="true" max="36" min="36" style="4" width="12.453125"/>
+    <col bestFit="true" customWidth="true" max="37" min="37" style="4" width="9.1796875"/>
+    <col bestFit="true" customWidth="true" max="38" min="38" style="4" width="10.1796875"/>
+    <col bestFit="true" customWidth="true" max="39" min="39" style="4" width="16.1796875"/>
     <col bestFit="true" customWidth="true" max="40" min="40" style="4" width="8"/>
-    <col bestFit="true" customWidth="true" max="41" min="41" style="4" width="8.140625"/>
-    <col bestFit="true" customWidth="true" max="42" min="42" style="4" width="9.85546875"/>
+    <col bestFit="true" customWidth="true" max="41" min="41" style="4" width="8.1796875"/>
+    <col bestFit="true" customWidth="true" max="42" min="42" style="4" width="9.81640625"/>
     <col bestFit="true" customWidth="true" max="43" min="43" style="4" width="8"/>
-    <col bestFit="true" customWidth="true" max="44" min="44" style="4" width="11.140625"/>
+    <col bestFit="true" customWidth="true" max="44" min="44" style="4" width="11.1796875"/>
     <col bestFit="true" customWidth="true" max="45" min="45" style="4" width="8"/>
-    <col bestFit="true" customWidth="true" max="46" min="46" style="4" width="18.28515625"/>
-    <col bestFit="true" customWidth="true" max="47" min="47" style="4" width="14.5703125"/>
-    <col bestFit="true" customWidth="true" max="48" min="48" style="4" width="13.7109375"/>
+    <col bestFit="true" customWidth="true" max="46" min="46" style="4" width="18.26953125"/>
+    <col bestFit="true" customWidth="true" max="47" min="47" style="4" width="14.54296875"/>
+    <col bestFit="true" customWidth="true" max="48" min="48" style="4" width="13.7265625"/>
     <col bestFit="true" customWidth="true" max="49" min="49" style="4" width="14"/>
-    <col bestFit="true" customWidth="true" max="50" min="50" style="4" width="14.7109375"/>
-    <col bestFit="true" customWidth="true" max="51" min="51" style="4" width="15.140625"/>
-    <col bestFit="true" customWidth="true" max="52" min="52" style="4" width="14.28515625"/>
-    <col bestFit="true" customWidth="true" max="53" min="53" style="4" width="14.5703125"/>
+    <col bestFit="true" customWidth="true" max="50" min="50" style="4" width="14.7265625"/>
+    <col bestFit="true" customWidth="true" max="51" min="51" style="4" width="15.1796875"/>
+    <col bestFit="true" customWidth="true" max="52" min="52" style="4" width="14.26953125"/>
+    <col bestFit="true" customWidth="true" max="53" min="53" style="4" width="14.54296875"/>
     <col bestFit="true" customWidth="true" max="54" min="54" style="4" width="8"/>
-    <col bestFit="true" customWidth="true" max="56" min="55" style="4" width="10.5703125"/>
-    <col bestFit="true" customWidth="true" max="57" min="57" style="4" width="6.28515625"/>
-    <col max="16384" min="58" style="4" width="12.5703125"/>
+    <col bestFit="true" customWidth="true" max="56" min="55" style="4" width="10.54296875"/>
+    <col bestFit="true" customWidth="true" max="57" min="57" style="4" width="6.26953125"/>
+    <col max="16384" min="58" style="4" width="12.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" s="3" customFormat="true">
+    <row r="1" spans="1:61" s="3" customFormat="true">
       <c r="A1" s="3">
         <v>0</v>
       </c>
@@ -1576,8 +2007,14 @@
       <c r="BG1" s="3">
         <v>58</v>
       </c>
-    </row>
-    <row r="2" spans="1:59" s="5" customFormat="true" ht="45">
+      <c r="BH1" s="3">
+        <v>59</v>
+      </c>
+      <c r="BI1" s="3">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:61" s="5" customFormat="true" ht="43.5">
       <c r="B2" s="5" t="s">
         <v>4</v>
       </c>
@@ -1752,8 +2189,14 @@
       <c r="BG2" s="5" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="3" spans="1:59" s="5" customFormat="true">
+      <c r="BH2" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="BI2" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:61" s="5" customFormat="true">
       <c r="B3" s="5">
         <v>0</v>
       </c>
@@ -1920,13 +2363,20 @@
       <c r="BG3" s="6">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:59">
+      <c r="BH3" s="5">
+        <v>0</v>
+      </c>
+      <c r="BI3" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:61">
       <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>128</v>
+      <c r="C4" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH4,Entities!$B$3:C104856,2,FALSE),"_",F4,"_",E4,"_",BI4)</f>
+        <v>OGANICA USA_2021_1_v1</v>
       </c>
       <c r="D4" s="5">
         <v>0</v>
@@ -2085,15 +2535,22 @@
         <v>0</v>
       </c>
       <c r="BG4" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:59">
+        <v>100</v>
+      </c>
+      <c r="BH4" s="7">
+        <v>3</v>
+      </c>
+      <c r="BI4" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:61">
       <c r="B5" s="4">
         <v>6</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>129</v>
+      <c r="C5" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH5,Entities!$B$3:C104857,2,FALSE),"_",F5,"_",E5,"_",BI5)</f>
+        <v>OGANICA EU_2021_1_v1</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="4">
@@ -2250,15 +2707,22 @@
         <v>0</v>
       </c>
       <c r="BG5" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:59">
+        <v>100</v>
+      </c>
+      <c r="BH5" s="7">
+        <v>6</v>
+      </c>
+      <c r="BI5" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="6" spans="1:61">
       <c r="B6" s="4">
         <v>1</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>132</v>
+      <c r="C6" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH6,Entities!$B$3:C104858,2,FALSE),"_",F6,"_",E6,"_",BI6)</f>
+        <v>Small Office_2021_1_v1</v>
       </c>
       <c r="D6" s="4">
         <v>3</v>
@@ -2282,37 +2746,37 @@
         <v>2035</v>
       </c>
       <c r="K6" s="4">
-        <v>0.055</v>
+        <v>0</v>
       </c>
       <c r="L6" s="4">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="M6" s="4">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="N6" s="4">
-        <v>0.019</v>
+        <v>0</v>
       </c>
       <c r="O6" s="4">
-        <v>0.044000000000000004</v>
+        <v>0</v>
       </c>
       <c r="P6" s="4">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="4">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="R6" s="4">
-        <v>0.025</v>
+        <v>0</v>
       </c>
       <c r="S6" s="4">
-        <v>0.0555</v>
+        <v>0</v>
       </c>
       <c r="T6" s="4">
-        <v>3.5</v>
+        <v>0</v>
       </c>
       <c r="V6" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="W6" s="4">
         <v>0</v>
@@ -2324,114 +2788,121 @@
         <v>0</v>
       </c>
       <c r="Z6" s="4">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="4">
-        <v>0.15</v>
+        <v>0</v>
       </c>
       <c r="AB6" s="4">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="4">
-        <v>0.021</v>
+        <v>0</v>
       </c>
       <c r="AD6" s="4">
-        <v>0.24</v>
+        <v>0</v>
       </c>
       <c r="AE6" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AF6" s="4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="AG6" s="4">
         <v>0</v>
       </c>
       <c r="AH6" s="4" t="s">
-        <v>59</v>
+        <v>112</v>
       </c>
       <c r="AI6" s="4">
-        <v>0.4</v>
+        <v>0</v>
       </c>
       <c r="AJ6" s="4">
         <v>0</v>
       </c>
       <c r="AK6" s="4">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="AL6" s="4">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="AM6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN6" s="4">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="AO6" s="4">
         <v>0</v>
       </c>
       <c r="AP6" s="4">
-        <v>1.2</v>
+        <v>0</v>
       </c>
       <c r="AQ6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR6" s="4">
         <v>0</v>
       </c>
       <c r="AS6" s="4">
-        <v>0.03</v>
+        <v>0</v>
       </c>
       <c r="AT6" s="4">
-        <v>0.0075</v>
+        <v>0</v>
       </c>
       <c r="AU6" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AV6" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AW6" s="4">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="AX6" s="4">
-        <v>0.0075</v>
+        <v>0</v>
       </c>
       <c r="AY6" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="AZ6" s="4">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="BA6" s="4">
-        <v>0.001</v>
+        <v>0</v>
       </c>
       <c r="BB6" s="4">
-        <v>0.0005</v>
+        <v>0</v>
       </c>
       <c r="BC6" s="4">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BD6" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BE6" s="4" t="s">
         <v>130</v>
       </c>
       <c r="BF6" s="4">
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="BG6" s="6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="7" spans="1:59">
+        <v>0</v>
+      </c>
+      <c r="BH6" s="7">
+        <v>1</v>
+      </c>
+      <c r="BI6" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="7" spans="1:61">
       <c r="B7" s="4">
         <v>4</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>133</v>
+      <c r="C7" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH7,Entities!$B$3:C104859,2,FALSE),"_",F7,"_",E7,"_",BI7)</f>
+        <v>Residential_2021_1_v1</v>
       </c>
       <c r="D7" s="4">
         <v>3</v>
@@ -2455,7 +2926,7 @@
         <v>2035</v>
       </c>
       <c r="K7" s="4">
-        <v>0.055</v>
+        <v>5.5E-2</v>
       </c>
       <c r="L7" s="4">
         <v>18</v>
@@ -2464,10 +2935,10 @@
         <v>18</v>
       </c>
       <c r="N7" s="4">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="O7" s="4">
-        <v>0.0285</v>
+        <v>2.8500000000000001E-2</v>
       </c>
       <c r="P7" s="4">
         <v>36</v>
@@ -2476,10 +2947,10 @@
         <v>24</v>
       </c>
       <c r="R7" s="4">
-        <v>0.022000000000000002</v>
+        <v>2.2000000000000002E-2</v>
       </c>
       <c r="S7" s="4">
-        <v>0.054000000000000006</v>
+        <v>5.4000000000000006E-2</v>
       </c>
       <c r="T7" s="4">
         <v>2</v>
@@ -2503,10 +2974,10 @@
         <v>0.15</v>
       </c>
       <c r="AB7" s="4">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="AC7" s="4">
-        <v>0.024</v>
+        <v>1.6E-2</v>
       </c>
       <c r="AD7" s="4">
         <v>0.16</v>
@@ -2551,13 +3022,13 @@
         <v>1.6</v>
       </c>
       <c r="AR7" s="4">
-        <v>0.027000000000000003</v>
+        <v>2.7000000000000003E-2</v>
       </c>
       <c r="AS7" s="4">
         <v>0</v>
       </c>
       <c r="AT7" s="4">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AU7" s="4">
         <v>6</v>
@@ -2566,10 +3037,10 @@
         <v>6</v>
       </c>
       <c r="AW7" s="4">
-        <v>0.0015</v>
+        <v>1.5E-3</v>
       </c>
       <c r="AX7" s="4">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AY7" s="4">
         <v>6</v>
@@ -2578,10 +3049,10 @@
         <v>6</v>
       </c>
       <c r="BA7" s="4">
-        <v>0.0015</v>
+        <v>1.5E-3</v>
       </c>
       <c r="BB7" s="4">
-        <v>0.004</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="BC7" s="4">
         <v>1</v>
@@ -2596,15 +3067,22 @@
         <v>1.25</v>
       </c>
       <c r="BG7" s="6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:59">
+        <v>100</v>
+      </c>
+      <c r="BH7" s="7">
+        <v>4</v>
+      </c>
+      <c r="BI7" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="8" spans="1:61">
       <c r="B8" s="4">
         <v>5</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>134</v>
+      <c r="C8" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH8,Entities!$B$3:C104860,2,FALSE),"_",F8,"_",E8,"_",BI8)</f>
+        <v>Light Industrial_2021_1_v1</v>
       </c>
       <c r="D8" s="4">
         <v>3</v>
@@ -2628,7 +3106,7 @@
         <v>2035</v>
       </c>
       <c r="K8" s="4">
-        <v>0.055</v>
+        <v>5.5E-2</v>
       </c>
       <c r="L8" s="4">
         <v>18</v>
@@ -2637,10 +3115,10 @@
         <v>18</v>
       </c>
       <c r="N8" s="4">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="O8" s="4">
-        <v>0.031</v>
+        <v>3.1E-2</v>
       </c>
       <c r="P8" s="4">
         <v>30</v>
@@ -2649,10 +3127,10 @@
         <v>24</v>
       </c>
       <c r="R8" s="4">
-        <v>0.0195</v>
+        <v>1.95E-2</v>
       </c>
       <c r="S8" s="4">
-        <v>0.054000000000000006</v>
+        <v>5.4000000000000006E-2</v>
       </c>
       <c r="T8" s="4">
         <v>2</v>
@@ -2676,10 +3154,10 @@
         <v>0.15</v>
       </c>
       <c r="AB8" s="4">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="AC8" s="4">
-        <v>0.024</v>
+        <v>1.6E-2</v>
       </c>
       <c r="AD8" s="4">
         <v>0.11</v>
@@ -2724,13 +3202,13 @@
         <v>1.5</v>
       </c>
       <c r="AR8" s="4">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AS8" s="4">
-        <v>0.013999999999999999</v>
+        <v>1.3999999999999999E-2</v>
       </c>
       <c r="AT8" s="4">
-        <v>0.004</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AU8" s="4">
         <v>6</v>
@@ -2739,10 +3217,10 @@
         <v>6</v>
       </c>
       <c r="AW8" s="4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="AX8" s="4">
-        <v>0.004</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="AY8" s="4">
         <v>6</v>
@@ -2751,10 +3229,10 @@
         <v>6</v>
       </c>
       <c r="BA8" s="4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="BB8" s="4">
-        <v>0.001</v>
+        <v>1E-3</v>
       </c>
       <c r="BC8" s="4">
         <v>3</v>
@@ -2769,15 +3247,22 @@
         <v>8</v>
       </c>
       <c r="BG8" s="6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:59">
+        <v>100</v>
+      </c>
+      <c r="BH8" s="7">
+        <v>5</v>
+      </c>
+      <c r="BI8" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="9" spans="1:61">
       <c r="B9" s="4">
         <v>11</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>135</v>
+      <c r="C9" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH9,Entities!$B$3:C104861,2,FALSE),"_",F9,"_",E9,"_",BI9)</f>
+        <v>Logistics_2021_1_v1</v>
       </c>
       <c r="D9" s="4">
         <v>3</v>
@@ -2801,7 +3286,7 @@
         <v>2035</v>
       </c>
       <c r="K9" s="4">
-        <v>0.055</v>
+        <v>5.5E-2</v>
       </c>
       <c r="L9" s="4">
         <v>18</v>
@@ -2810,10 +3295,10 @@
         <v>18</v>
       </c>
       <c r="N9" s="4">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="O9" s="4">
-        <v>0.034</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="P9" s="4">
         <v>32</v>
@@ -2822,10 +3307,10 @@
         <v>24</v>
       </c>
       <c r="R9" s="4">
-        <v>0.0215</v>
+        <v>2.1499999999999998E-2</v>
       </c>
       <c r="S9" s="4">
-        <v>0.049</v>
+        <v>4.9000000000000002E-2</v>
       </c>
       <c r="T9" s="4">
         <v>3.3</v>
@@ -2849,13 +3334,13 @@
         <v>0.15</v>
       </c>
       <c r="AB9" s="4">
-        <v>0.5</v>
+        <v>0.65</v>
       </c>
       <c r="AC9" s="4">
-        <v>0.026000000000000002</v>
+        <v>1.6E-2</v>
       </c>
       <c r="AD9" s="4">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="AE9" s="4">
         <v>1</v>
@@ -2900,10 +3385,10 @@
         <v>0</v>
       </c>
       <c r="AS9" s="4">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AT9" s="4">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AU9" s="4">
         <v>6</v>
@@ -2912,10 +3397,10 @@
         <v>6</v>
       </c>
       <c r="AW9" s="4">
-        <v>0.0015</v>
+        <v>1.5E-3</v>
       </c>
       <c r="AX9" s="4">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="AY9" s="4">
         <v>6</v>
@@ -2924,10 +3409,10 @@
         <v>6</v>
       </c>
       <c r="BA9" s="4">
-        <v>0.0015</v>
+        <v>1.5E-3</v>
       </c>
       <c r="BB9" s="4">
-        <v>0.0005</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="BC9" s="4">
         <v>6</v>
@@ -2942,15 +3427,22 @@
         <v>2.9</v>
       </c>
       <c r="BG9" s="6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="10" spans="1:59">
+        <v>100</v>
+      </c>
+      <c r="BH9" s="7">
+        <v>11</v>
+      </c>
+      <c r="BI9" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="10" spans="1:61">
       <c r="B10" s="4">
         <v>2</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>122</v>
+      <c r="C10" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH10,Entities!$B$3:C104862,2,FALSE),"_",F10,"_",E10,"_",BI10)</f>
+        <v>Industrial 1_2021_1_v1</v>
       </c>
       <c r="D10" s="4">
         <v>6</v>
@@ -2983,10 +3475,10 @@
         <v>24</v>
       </c>
       <c r="N10" s="4">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="O10" s="4">
-        <v>0.035</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="P10" s="4">
         <v>18</v>
@@ -2995,16 +3487,16 @@
         <v>18</v>
       </c>
       <c r="R10" s="4">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
       <c r="S10" s="4">
-        <v>0.055</v>
+        <v>5.5E-2</v>
       </c>
       <c r="T10" s="4">
         <v>4</v>
       </c>
       <c r="V10" s="4">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="W10" s="4">
         <v>0</v>
@@ -3046,7 +3538,7 @@
         <v>0</v>
       </c>
       <c r="AJ10" s="4">
-        <v>0.0175</v>
+        <v>1.7500000000000002E-2</v>
       </c>
       <c r="AK10" s="4">
         <v>9</v>
@@ -3070,13 +3562,13 @@
         <v>1.6</v>
       </c>
       <c r="AR10" s="4">
-        <v>0.027000000000000003</v>
+        <v>2.7000000000000003E-2</v>
       </c>
       <c r="AS10" s="4">
-        <v>0.0075</v>
+        <v>7.4999999999999997E-3</v>
       </c>
       <c r="AT10" s="4">
-        <v>0.0125</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="AU10" s="4">
         <v>6</v>
@@ -3085,22 +3577,22 @@
         <v>4</v>
       </c>
       <c r="AW10" s="4">
-        <v>0.0015</v>
+        <v>1.5E-3</v>
       </c>
       <c r="AX10" s="4">
-        <v>0.01</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="AY10" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AZ10" s="4">
         <v>4</v>
       </c>
       <c r="BA10" s="4">
-        <v>0.0015</v>
+        <v>1.5E-3</v>
       </c>
       <c r="BB10" s="4">
-        <v>0.0005</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="BC10" s="4">
         <v>0</v>
@@ -3115,15 +3607,22 @@
         <v>1.6</v>
       </c>
       <c r="BG10" s="6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:59">
+        <v>100</v>
+      </c>
+      <c r="BH10" s="7">
+        <v>2</v>
+      </c>
+      <c r="BI10" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:61">
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>114</v>
+      <c r="C11" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH11,Entities!$B$3:C104863,2,FALSE),"_",F11,"_",E11,"_",BI11)</f>
+        <v>Industrial 2_2021_1_v1</v>
       </c>
       <c r="D11" s="4">
         <v>6</v>
@@ -3288,15 +3787,22 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="BG11" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:59">
+        <v>100</v>
+      </c>
+      <c r="BH11" s="7">
+        <v>7</v>
+      </c>
+      <c r="BI11" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="12" spans="1:61">
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="4" t="s">
-        <v>115</v>
+      <c r="C12" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH12,Entities!$B$3:C104864,2,FALSE),"_",F12,"_",E12,"_",BI12)</f>
+        <v>Industrial 3_2021_1_v1</v>
       </c>
       <c r="D12" s="4">
         <v>6</v>
@@ -3320,7 +3826,7 @@
         <v>2035</v>
       </c>
       <c r="K12" s="4">
-        <v>0.055</v>
+        <v>5.5E-2</v>
       </c>
       <c r="L12" s="4">
         <v>18</v>
@@ -3329,10 +3835,10 @@
         <v>18</v>
       </c>
       <c r="N12" s="4">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="O12" s="4">
-        <v>0.017</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="P12" s="4">
         <v>36</v>
@@ -3341,7 +3847,7 @@
         <v>24</v>
       </c>
       <c r="R12" s="4">
-        <v>0.013999999999999999</v>
+        <v>1.3999999999999999E-2</v>
       </c>
       <c r="S12" s="4">
         <v>0.05</v>
@@ -3392,7 +3898,7 @@
         <v>0</v>
       </c>
       <c r="AJ12" s="4">
-        <v>0.018500000000000003</v>
+        <v>1.8500000000000003E-2</v>
       </c>
       <c r="AK12" s="4">
         <v>12</v>
@@ -3416,13 +3922,13 @@
         <v>1.5</v>
       </c>
       <c r="AR12" s="4">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AS12" s="4">
-        <v>0.0125</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="AT12" s="4">
-        <v>0.006999999999999999</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="AU12" s="4">
         <v>6</v>
@@ -3431,10 +3937,10 @@
         <v>6</v>
       </c>
       <c r="AW12" s="4">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="AX12" s="4">
-        <v>0.006999999999999999</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="AY12" s="4">
         <v>6</v>
@@ -3443,10 +3949,10 @@
         <v>6</v>
       </c>
       <c r="BA12" s="4">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="BB12" s="4">
-        <v>0.0005</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="BC12" s="4">
         <v>4</v>
@@ -3461,15 +3967,22 @@
         <v>0.8</v>
       </c>
       <c r="BG12" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:59">
+        <v>100</v>
+      </c>
+      <c r="BH12" s="7">
+        <v>8</v>
+      </c>
+      <c r="BI12" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="13" spans="1:61">
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>116</v>
+      <c r="C13" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH13,Entities!$B$3:C104865,2,FALSE),"_",F13,"_",E13,"_",BI13)</f>
+        <v>Industrial 4_2021_1_v1</v>
       </c>
       <c r="D13" s="4">
         <v>6</v>
@@ -3493,7 +4006,7 @@
         <v>2035</v>
       </c>
       <c r="K13" s="4">
-        <v>0.055</v>
+        <v>5.5E-2</v>
       </c>
       <c r="L13" s="4">
         <v>18</v>
@@ -3502,7 +4015,7 @@
         <v>18</v>
       </c>
       <c r="N13" s="4">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="O13" s="4">
         <v>0</v>
@@ -3514,16 +4027,16 @@
         <v>12</v>
       </c>
       <c r="R13" s="4">
-        <v>0.012</v>
+        <v>1.2E-2</v>
       </c>
       <c r="S13" s="4">
-        <v>0.084</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="T13" s="4">
         <v>2.5</v>
       </c>
       <c r="V13" s="4">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="W13" s="4">
         <v>0</v>
@@ -3565,7 +4078,7 @@
         <v>0.4</v>
       </c>
       <c r="AJ13" s="4">
-        <v>0.0149</v>
+        <v>1.49E-2</v>
       </c>
       <c r="AK13" s="4">
         <v>12</v>
@@ -3589,13 +4102,13 @@
         <v>1.5</v>
       </c>
       <c r="AR13" s="4">
-        <v>0.025</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="AS13" s="4">
-        <v>0.0125</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="AT13" s="4">
-        <v>0.006999999999999999</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="AU13" s="4">
         <v>6</v>
@@ -3604,10 +4117,10 @@
         <v>6</v>
       </c>
       <c r="AW13" s="4">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="AX13" s="4">
-        <v>0.006999999999999999</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="AY13" s="4">
         <v>6</v>
@@ -3616,10 +4129,10 @@
         <v>6</v>
       </c>
       <c r="BA13" s="4">
-        <v>0.0025</v>
+        <v>2.5000000000000001E-3</v>
       </c>
       <c r="BB13" s="4">
-        <v>0.0001</v>
+        <v>1E-4</v>
       </c>
       <c r="BC13" s="4">
         <v>0</v>
@@ -3634,15 +4147,22 @@
         <v>0.8</v>
       </c>
       <c r="BG13" s="6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:59">
+        <v>100</v>
+      </c>
+      <c r="BH13" s="7">
+        <v>9</v>
+      </c>
+      <c r="BI13" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="14" spans="1:61">
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="4" t="s">
-        <v>117</v>
+      <c r="C14" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH14,Entities!$B$3:C104866,2,FALSE),"_",F14,"_",E14,"_",BI14)</f>
+        <v>Industrial 5_2021_1_v1</v>
       </c>
       <c r="D14" s="4">
         <v>6</v>
@@ -3666,7 +4186,7 @@
         <v>2035</v>
       </c>
       <c r="K14" s="4">
-        <v>0.055</v>
+        <v>5.5E-2</v>
       </c>
       <c r="L14" s="4">
         <v>18</v>
@@ -3675,10 +4195,10 @@
         <v>18</v>
       </c>
       <c r="N14" s="4">
-        <v>0.019</v>
+        <v>1.9E-2</v>
       </c>
       <c r="O14" s="4">
-        <v>0.021</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="P14" s="4">
         <v>36</v>
@@ -3687,7 +4207,7 @@
         <v>24</v>
       </c>
       <c r="R14" s="4">
-        <v>0.0175</v>
+        <v>1.7500000000000002E-2</v>
       </c>
       <c r="S14" s="4">
         <v>0.06</v>
@@ -3738,7 +4258,7 @@
         <v>0.4</v>
       </c>
       <c r="AJ14" s="4">
-        <v>0.015</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="AK14" s="4">
         <v>9</v>
@@ -3762,13 +4282,13 @@
         <v>1.5</v>
       </c>
       <c r="AR14" s="4">
-        <v>0.035</v>
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="AS14" s="4">
-        <v>0.0125</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="AT14" s="4">
-        <v>0.006999999999999999</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="AU14" s="4">
         <v>6</v>
@@ -3777,10 +4297,10 @@
         <v>6</v>
       </c>
       <c r="AW14" s="4">
-        <v>0.0015</v>
+        <v>1.5E-3</v>
       </c>
       <c r="AX14" s="4">
-        <v>0.006999999999999999</v>
+        <v>6.9999999999999993E-3</v>
       </c>
       <c r="AY14" s="4">
         <v>6</v>
@@ -3789,10 +4309,10 @@
         <v>6</v>
       </c>
       <c r="BA14" s="4">
-        <v>0.0015</v>
+        <v>1.5E-3</v>
       </c>
       <c r="BB14" s="4">
-        <v>0.0005</v>
+        <v>5.0000000000000001E-4</v>
       </c>
       <c r="BC14" s="4">
         <v>3</v>
@@ -3808,6 +4328,906 @@
       </c>
       <c r="BG14" s="6">
         <v>100</v>
+      </c>
+      <c r="BH14" s="7">
+        <v>10</v>
+      </c>
+      <c r="BI14" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:61">
+      <c r="B15" s="4">
+        <v>12</v>
+      </c>
+      <c r="C15" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH15,Entities!$B$3:C104867,2,FALSE),"_",F15,"_",E15,"_",BI15)</f>
+        <v>OGANICA USA_2022_1_v1</v>
+      </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4">
+        <v>2022</v>
+      </c>
+      <c r="G15" s="4">
+        <v>12</v>
+      </c>
+      <c r="H15" s="4">
+        <v>2030</v>
+      </c>
+      <c r="I15" s="4">
+        <v>12</v>
+      </c>
+      <c r="J15" s="4">
+        <v>2035</v>
+      </c>
+      <c r="K15" s="4">
+        <v>0</v>
+      </c>
+      <c r="L15" s="4">
+        <v>0</v>
+      </c>
+      <c r="M15" s="4">
+        <v>0</v>
+      </c>
+      <c r="N15" s="4">
+        <v>0</v>
+      </c>
+      <c r="O15" s="4">
+        <v>0</v>
+      </c>
+      <c r="P15" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="4">
+        <v>0</v>
+      </c>
+      <c r="R15" s="4">
+        <v>0</v>
+      </c>
+      <c r="S15" s="4">
+        <v>0</v>
+      </c>
+      <c r="T15" s="4">
+        <v>0</v>
+      </c>
+      <c r="V15" s="4">
+        <v>9</v>
+      </c>
+      <c r="W15" s="4">
+        <v>0</v>
+      </c>
+      <c r="X15" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AF15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AG15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH15" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AJ15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AL15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AM15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AN15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AO15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AQ15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AR15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AU15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AV15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AW15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AX15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AY15" s="4">
+        <v>0</v>
+      </c>
+      <c r="AZ15" s="4">
+        <v>0</v>
+      </c>
+      <c r="BA15" s="4">
+        <v>0</v>
+      </c>
+      <c r="BC15" s="4">
+        <v>0</v>
+      </c>
+      <c r="BD15" s="4">
+        <v>0</v>
+      </c>
+      <c r="BE15" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="BF15" s="4">
+        <v>0</v>
+      </c>
+      <c r="BG15" s="6">
+        <v>100</v>
+      </c>
+      <c r="BH15" s="7">
+        <v>3</v>
+      </c>
+      <c r="BI15" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="16" spans="1:61">
+      <c r="B16" s="4">
+        <v>13</v>
+      </c>
+      <c r="C16" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH16,Entities!$B$3:C104868,2,FALSE),"_",F16,"_",E16,"_",BI16)</f>
+        <v>Small Office_2022_1_v1</v>
+      </c>
+      <c r="D16" s="4">
+        <v>12</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4">
+        <v>2022</v>
+      </c>
+      <c r="G16" s="4">
+        <v>12</v>
+      </c>
+      <c r="H16" s="4">
+        <v>2030</v>
+      </c>
+      <c r="I16" s="4">
+        <v>12</v>
+      </c>
+      <c r="J16" s="4">
+        <v>2035</v>
+      </c>
+      <c r="K16" s="4">
+        <v>0.085</v>
+      </c>
+      <c r="L16" s="4">
+        <v>18</v>
+      </c>
+      <c r="M16" s="4">
+        <v>18</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0.019</v>
+      </c>
+      <c r="O16" s="4">
+        <v>0.044000000000000004</v>
+      </c>
+      <c r="P16" s="4">
+        <v>18</v>
+      </c>
+      <c r="Q16" s="4">
+        <v>18</v>
+      </c>
+      <c r="R16" s="4">
+        <v>0.025</v>
+      </c>
+      <c r="S16" s="4">
+        <v>0.0555</v>
+      </c>
+      <c r="T16" s="4">
+        <v>3.5</v>
+      </c>
+      <c r="V16" s="4">
+        <v>9</v>
+      </c>
+      <c r="W16" s="4">
+        <v>0</v>
+      </c>
+      <c r="X16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="4">
+        <v>39</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="AB16" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="AC16" s="4">
+        <v>0.016</v>
+      </c>
+      <c r="AD16" s="4">
+        <v>0.24</v>
+      </c>
+      <c r="AE16" s="4">
+        <v>10</v>
+      </c>
+      <c r="AF16" s="4">
+        <v>10</v>
+      </c>
+      <c r="AG16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH16" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI16" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="AJ16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK16" s="4">
+        <v>9</v>
+      </c>
+      <c r="AL16" s="4">
+        <v>60</v>
+      </c>
+      <c r="AM16" s="4">
+        <v>1</v>
+      </c>
+      <c r="AN16" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="AO16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP16" s="4">
+        <v>1.2</v>
+      </c>
+      <c r="AQ16" s="4">
+        <v>1</v>
+      </c>
+      <c r="AR16" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS16" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="AT16" s="4">
+        <v>0.0075</v>
+      </c>
+      <c r="AU16" s="4">
+        <v>5</v>
+      </c>
+      <c r="AV16" s="4">
+        <v>5</v>
+      </c>
+      <c r="AW16" s="4">
+        <v>0.001</v>
+      </c>
+      <c r="AX16" s="4">
+        <v>0.0075</v>
+      </c>
+      <c r="AY16" s="4">
+        <v>5</v>
+      </c>
+      <c r="AZ16" s="4">
+        <v>5</v>
+      </c>
+      <c r="BA16" s="4">
+        <v>0.001</v>
+      </c>
+      <c r="BB16" s="4">
+        <v>0.0005</v>
+      </c>
+      <c r="BC16" s="4">
+        <v>3</v>
+      </c>
+      <c r="BD16" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE16" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="BF16" s="4">
+        <v>14</v>
+      </c>
+      <c r="BG16" s="6">
+        <v>1000</v>
+      </c>
+      <c r="BH16" s="7">
+        <v>1</v>
+      </c>
+      <c r="BI16" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="17" spans="2:61">
+      <c r="B17" s="4">
+        <v>14</v>
+      </c>
+      <c r="C17" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH17,Entities!$B$3:C104869,2,FALSE),"_",F17,"_",E17,"_",BI17)</f>
+        <v>Residential_2022_1_v1</v>
+      </c>
+      <c r="D17" s="4">
+        <v>12</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4">
+        <v>2022</v>
+      </c>
+      <c r="G17" s="4">
+        <v>12</v>
+      </c>
+      <c r="H17" s="4">
+        <v>2030</v>
+      </c>
+      <c r="I17" s="4">
+        <v>12</v>
+      </c>
+      <c r="J17" s="4">
+        <v>2035</v>
+      </c>
+      <c r="K17" s="4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="L17" s="4">
+        <v>18</v>
+      </c>
+      <c r="M17" s="4">
+        <v>18</v>
+      </c>
+      <c r="N17" s="4">
+        <v>1.9E-2</v>
+      </c>
+      <c r="O17" s="4">
+        <v>2.8500000000000001E-2</v>
+      </c>
+      <c r="P17" s="4">
+        <v>36</v>
+      </c>
+      <c r="Q17" s="4">
+        <v>24</v>
+      </c>
+      <c r="R17" s="4">
+        <v>2.2000000000000002E-2</v>
+      </c>
+      <c r="S17" s="4">
+        <v>5.4000000000000006E-2</v>
+      </c>
+      <c r="T17" s="4">
+        <v>2</v>
+      </c>
+      <c r="V17" s="4">
+        <v>9</v>
+      </c>
+      <c r="W17" s="4">
+        <v>0</v>
+      </c>
+      <c r="X17" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="4">
+        <v>28</v>
+      </c>
+      <c r="AA17" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="AB17" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="AC17" s="4">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AD17" s="4">
+        <v>0.16</v>
+      </c>
+      <c r="AE17" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF17" s="4">
+        <v>6</v>
+      </c>
+      <c r="AG17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI17" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="AJ17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK17" s="4">
+        <v>3</v>
+      </c>
+      <c r="AL17" s="4">
+        <v>12</v>
+      </c>
+      <c r="AM17" s="4">
+        <v>1</v>
+      </c>
+      <c r="AN17" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="AO17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP17" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="AQ17" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="AR17" s="4">
+        <v>2.7000000000000003E-2</v>
+      </c>
+      <c r="AS17" s="4">
+        <v>0</v>
+      </c>
+      <c r="AT17" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AU17" s="4">
+        <v>6</v>
+      </c>
+      <c r="AV17" s="4">
+        <v>6</v>
+      </c>
+      <c r="AW17" s="4">
+        <v>1.5E-3</v>
+      </c>
+      <c r="AX17" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AY17" s="4">
+        <v>6</v>
+      </c>
+      <c r="AZ17" s="4">
+        <v>6</v>
+      </c>
+      <c r="BA17" s="4">
+        <v>1.5E-3</v>
+      </c>
+      <c r="BB17" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="BC17" s="4">
+        <v>1</v>
+      </c>
+      <c r="BD17" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE17" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="BF17" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="BG17" s="6">
+        <v>100</v>
+      </c>
+      <c r="BH17" s="7">
+        <v>4</v>
+      </c>
+      <c r="BI17" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="18" spans="2:61">
+      <c r="B18" s="4">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH18,Entities!$B$3:C104870,2,FALSE),"_",F18,"_",E18,"_",BI18)</f>
+        <v>Light Industrial_2022_1_v1</v>
+      </c>
+      <c r="D18" s="4">
+        <v>12</v>
+      </c>
+      <c r="E18" s="4">
+        <v>1</v>
+      </c>
+      <c r="F18" s="4">
+        <v>2022</v>
+      </c>
+      <c r="G18" s="4">
+        <v>12</v>
+      </c>
+      <c r="H18" s="4">
+        <v>2030</v>
+      </c>
+      <c r="I18" s="4">
+        <v>12</v>
+      </c>
+      <c r="J18" s="4">
+        <v>2035</v>
+      </c>
+      <c r="K18" s="4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="L18" s="4">
+        <v>18</v>
+      </c>
+      <c r="M18" s="4">
+        <v>18</v>
+      </c>
+      <c r="N18" s="4">
+        <v>1.9E-2</v>
+      </c>
+      <c r="O18" s="4">
+        <v>3.1E-2</v>
+      </c>
+      <c r="P18" s="4">
+        <v>30</v>
+      </c>
+      <c r="Q18" s="4">
+        <v>24</v>
+      </c>
+      <c r="R18" s="4">
+        <v>1.95E-2</v>
+      </c>
+      <c r="S18" s="4">
+        <v>5.4000000000000006E-2</v>
+      </c>
+      <c r="T18" s="4">
+        <v>2</v>
+      </c>
+      <c r="V18" s="4">
+        <v>9</v>
+      </c>
+      <c r="W18" s="4">
+        <v>0</v>
+      </c>
+      <c r="X18" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="4">
+        <v>39</v>
+      </c>
+      <c r="AA18" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="AB18" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="AC18" s="4">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AD18" s="4">
+        <v>0.11</v>
+      </c>
+      <c r="AE18" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF18" s="4">
+        <v>6</v>
+      </c>
+      <c r="AG18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH18" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI18" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="AJ18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK18" s="4">
+        <v>6</v>
+      </c>
+      <c r="AL18" s="4">
+        <v>60</v>
+      </c>
+      <c r="AM18" s="4">
+        <v>1</v>
+      </c>
+      <c r="AN18" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="AO18" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP18" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="AQ18" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="AR18" s="4">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="AS18" s="4">
+        <v>1.3999999999999999E-2</v>
+      </c>
+      <c r="AT18" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AU18" s="4">
+        <v>6</v>
+      </c>
+      <c r="AV18" s="4">
+        <v>6</v>
+      </c>
+      <c r="AW18" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="AX18" s="4">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AY18" s="4">
+        <v>6</v>
+      </c>
+      <c r="AZ18" s="4">
+        <v>6</v>
+      </c>
+      <c r="BA18" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="BB18" s="4">
+        <v>1E-3</v>
+      </c>
+      <c r="BC18" s="4">
+        <v>3</v>
+      </c>
+      <c r="BD18" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE18" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="BF18" s="4">
+        <v>8</v>
+      </c>
+      <c r="BG18" s="6">
+        <v>100</v>
+      </c>
+      <c r="BH18" s="7">
+        <v>5</v>
+      </c>
+      <c r="BI18" s="5" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="19" spans="2:61">
+      <c r="B19" s="4">
+        <v>16</v>
+      </c>
+      <c r="C19" s="4" t="str">
+        <f>_xlfn.CONCAT(VLOOKUP(BH19,Entities!$B$3:C104871,2,FALSE),"_",F19,"_",E19,"_",BI19)</f>
+        <v>Logistics_2022_1_v1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>12</v>
+      </c>
+      <c r="E19" s="4">
+        <v>1</v>
+      </c>
+      <c r="F19" s="4">
+        <v>2022</v>
+      </c>
+      <c r="G19" s="4">
+        <v>12</v>
+      </c>
+      <c r="H19" s="4">
+        <v>2030</v>
+      </c>
+      <c r="I19" s="4">
+        <v>12</v>
+      </c>
+      <c r="J19" s="4">
+        <v>2035</v>
+      </c>
+      <c r="K19" s="4">
+        <v>5.5E-2</v>
+      </c>
+      <c r="L19" s="4">
+        <v>18</v>
+      </c>
+      <c r="M19" s="4">
+        <v>18</v>
+      </c>
+      <c r="N19" s="4">
+        <v>1.9E-2</v>
+      </c>
+      <c r="O19" s="4">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="P19" s="4">
+        <v>32</v>
+      </c>
+      <c r="Q19" s="4">
+        <v>24</v>
+      </c>
+      <c r="R19" s="4">
+        <v>2.1499999999999998E-2</v>
+      </c>
+      <c r="S19" s="4">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="T19" s="4">
+        <v>3.3</v>
+      </c>
+      <c r="V19" s="4">
+        <v>9</v>
+      </c>
+      <c r="W19" s="4">
+        <v>0</v>
+      </c>
+      <c r="X19" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="4">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="4">
+        <v>39</v>
+      </c>
+      <c r="AA19" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="AB19" s="4">
+        <v>0.65</v>
+      </c>
+      <c r="AC19" s="4">
+        <v>1.6E-2</v>
+      </c>
+      <c r="AD19" s="4">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AE19" s="4">
+        <v>1</v>
+      </c>
+      <c r="AF19" s="4">
+        <v>6</v>
+      </c>
+      <c r="AG19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AH19" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="AI19" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="AJ19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AK19" s="4">
+        <v>8</v>
+      </c>
+      <c r="AL19" s="4">
+        <v>60</v>
+      </c>
+      <c r="AM19" s="4">
+        <v>1</v>
+      </c>
+      <c r="AN19" s="4">
+        <v>1</v>
+      </c>
+      <c r="AO19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AP19" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="AQ19" s="4">
+        <v>1.6</v>
+      </c>
+      <c r="AR19" s="4">
+        <v>0</v>
+      </c>
+      <c r="AS19" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AT19" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AU19" s="4">
+        <v>6</v>
+      </c>
+      <c r="AV19" s="4">
+        <v>6</v>
+      </c>
+      <c r="AW19" s="4">
+        <v>1.5E-3</v>
+      </c>
+      <c r="AX19" s="4">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AY19" s="4">
+        <v>6</v>
+      </c>
+      <c r="AZ19" s="4">
+        <v>6</v>
+      </c>
+      <c r="BA19" s="4">
+        <v>1.5E-3</v>
+      </c>
+      <c r="BB19" s="4">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="BC19" s="4">
+        <v>6</v>
+      </c>
+      <c r="BD19" s="4">
+        <v>1</v>
+      </c>
+      <c r="BE19" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="BF19" s="4">
+        <v>2.9</v>
+      </c>
+      <c r="BG19" s="6">
+        <v>100</v>
+      </c>
+      <c r="BH19" s="7">
+        <v>11</v>
+      </c>
+      <c r="BI19" s="5" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -3815,42 +5235,45 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:X34"/>
+  <dimension ref="A1:X59"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A33" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D59" sqref="D59"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="45.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="45.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.26953125" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.26953125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="45.85546875" style="1"/>
+    <col min="10" max="10" width="20.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="17.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="16384" width="45.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.35">
       <c r="A1" s="1">
         <v>0</v>
       </c>
@@ -3924,7 +5347,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
@@ -3995,7 +5418,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B3" s="1">
         <v>1</v>
       </c>
@@ -4034,7 +5457,7 @@
       </c>
       <c r="X3" s="2"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B4" s="1">
         <v>2</v>
       </c>
@@ -4073,7 +5496,7 @@
       </c>
       <c r="X4" s="2"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -4112,7 +5535,7 @@
       </c>
       <c r="X5" s="2"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -4151,7 +5574,7 @@
       </c>
       <c r="X6" s="2"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -4190,7 +5613,7 @@
       </c>
       <c r="X7" s="2"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -4229,7 +5652,7 @@
       </c>
       <c r="X8" s="2"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
         <v>7</v>
       </c>
@@ -4268,7 +5691,7 @@
       </c>
       <c r="X9" s="2"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B10" s="1">
         <v>8</v>
       </c>
@@ -4307,7 +5730,7 @@
       </c>
       <c r="X10" s="2"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
         <v>9</v>
       </c>
@@ -4345,7 +5768,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B12" s="1">
         <v>10</v>
       </c>
@@ -4383,7 +5806,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B13" s="1">
         <v>11</v>
       </c>
@@ -4422,7 +5845,7 @@
       </c>
       <c r="X13" s="2"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
         <v>12</v>
       </c>
@@ -4460,7 +5883,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B15" s="1">
         <v>13</v>
       </c>
@@ -4498,7 +5921,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.35">
       <c r="B16" s="1">
         <v>14</v>
       </c>
@@ -4536,7 +5959,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B17" s="1">
         <v>15</v>
       </c>
@@ -4574,7 +5997,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B18" s="1">
         <v>16</v>
       </c>
@@ -4612,7 +6035,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B19" s="1">
         <v>17</v>
       </c>
@@ -4650,7 +6073,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
         <v>18</v>
       </c>
@@ -4688,7 +6111,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B21" s="1">
         <v>19</v>
       </c>
@@ -4726,7 +6149,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="22" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B22" s="1">
         <v>20</v>
       </c>
@@ -4764,7 +6187,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B23" s="1">
         <v>21</v>
       </c>
@@ -4802,7 +6225,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B24" s="1">
         <v>22</v>
       </c>
@@ -4840,7 +6263,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B25" s="1">
         <v>23</v>
       </c>
@@ -4878,7 +6301,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B26" s="1">
         <v>24</v>
       </c>
@@ -4916,7 +6339,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B27" s="1">
         <v>25</v>
       </c>
@@ -4954,7 +6377,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="28" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B28" s="1">
         <v>26</v>
       </c>
@@ -4992,7 +6415,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B29" s="1">
         <v>27</v>
       </c>
@@ -5030,7 +6453,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B30" s="1">
         <v>28</v>
       </c>
@@ -5068,7 +6491,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B31" s="1">
         <v>29</v>
       </c>
@@ -5106,7 +6529,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:23" x14ac:dyDescent="0.35">
       <c r="B32" s="1">
         <v>30</v>
       </c>
@@ -5144,7 +6567,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B33" s="1">
         <v>31</v>
       </c>
@@ -5182,7 +6605,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:24" x14ac:dyDescent="0.35">
       <c r="B34" s="1">
         <v>32</v>
       </c>
@@ -5218,6 +6641,964 @@
       </c>
       <c r="W34" s="1">
         <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B35" s="1">
+        <v>33</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D35" s="1">
+        <v>13</v>
+      </c>
+      <c r="E35" s="1">
+        <v>11</v>
+      </c>
+      <c r="F35" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G35" s="1">
+        <v>12</v>
+      </c>
+      <c r="H35" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="K35" s="1">
+        <v>300000</v>
+      </c>
+      <c r="V35" s="1">
+        <v>10000</v>
+      </c>
+      <c r="W35" s="1">
+        <v>30</v>
+      </c>
+      <c r="X35" s="2"/>
+    </row>
+    <row r="36" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B36" s="1">
+        <v>34</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="1">
+        <v>13</v>
+      </c>
+      <c r="E36" s="1">
+        <v>11</v>
+      </c>
+      <c r="F36" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G36" s="1">
+        <v>12</v>
+      </c>
+      <c r="H36" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="K36" s="1">
+        <v>300000</v>
+      </c>
+      <c r="V36" s="1">
+        <v>10000</v>
+      </c>
+      <c r="W36" s="1">
+        <v>30</v>
+      </c>
+      <c r="X36" s="2"/>
+    </row>
+    <row r="37" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B37" s="1">
+        <v>35</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D37" s="1">
+        <v>13</v>
+      </c>
+      <c r="E37" s="1">
+        <v>2</v>
+      </c>
+      <c r="F37" s="1">
+        <v>2017</v>
+      </c>
+      <c r="G37" s="1">
+        <v>1</v>
+      </c>
+      <c r="H37" s="1">
+        <v>2022</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K37" s="1">
+        <v>175500</v>
+      </c>
+      <c r="V37" s="1">
+        <v>5900</v>
+      </c>
+      <c r="W37" s="1">
+        <v>30</v>
+      </c>
+      <c r="X37" s="2"/>
+    </row>
+    <row r="38" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B38" s="1">
+        <v>36</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D38" s="1">
+        <v>13</v>
+      </c>
+      <c r="E38" s="1">
+        <v>4</v>
+      </c>
+      <c r="F38" s="1">
+        <v>2016</v>
+      </c>
+      <c r="G38" s="1">
+        <v>3</v>
+      </c>
+      <c r="H38" s="1">
+        <v>2024</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K38" s="1">
+        <v>219000</v>
+      </c>
+      <c r="V38" s="1">
+        <v>7300</v>
+      </c>
+      <c r="W38" s="1">
+        <v>30</v>
+      </c>
+      <c r="X38" s="2"/>
+    </row>
+    <row r="39" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B39" s="1">
+        <v>37</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D39" s="1">
+        <v>13</v>
+      </c>
+      <c r="E39" s="1">
+        <v>10</v>
+      </c>
+      <c r="F39" s="1">
+        <v>2015</v>
+      </c>
+      <c r="G39" s="1">
+        <v>9</v>
+      </c>
+      <c r="H39" s="1">
+        <v>2025</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="K39" s="1">
+        <v>211500</v>
+      </c>
+      <c r="V39" s="1">
+        <v>7300</v>
+      </c>
+      <c r="W39" s="1">
+        <v>30</v>
+      </c>
+      <c r="X39" s="2"/>
+    </row>
+    <row r="40" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B40" s="1">
+        <v>38</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D40" s="1">
+        <v>13</v>
+      </c>
+      <c r="E40" s="1">
+        <v>5</v>
+      </c>
+      <c r="F40" s="1">
+        <v>2014</v>
+      </c>
+      <c r="G40" s="1">
+        <v>4</v>
+      </c>
+      <c r="H40" s="1">
+        <v>2026</v>
+      </c>
+      <c r="I40" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="K40" s="1">
+        <v>345000</v>
+      </c>
+      <c r="V40" s="1">
+        <v>11500</v>
+      </c>
+      <c r="W40" s="1">
+        <v>30</v>
+      </c>
+      <c r="X40" s="2"/>
+    </row>
+    <row r="41" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B41" s="1">
+        <v>39</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="1">
+        <v>13</v>
+      </c>
+      <c r="E41" s="1">
+        <v>0</v>
+      </c>
+      <c r="F41" s="1">
+        <v>0</v>
+      </c>
+      <c r="G41" s="1">
+        <v>0</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0</v>
+      </c>
+      <c r="I41" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K41" s="1">
+        <v>0</v>
+      </c>
+      <c r="V41" s="1">
+        <v>10000</v>
+      </c>
+      <c r="W41" s="1">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="42" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B42" s="1">
+        <v>40</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D42" s="1">
+        <v>13</v>
+      </c>
+      <c r="E42" s="1">
+        <v>0</v>
+      </c>
+      <c r="F42" s="1">
+        <v>0</v>
+      </c>
+      <c r="G42" s="1">
+        <v>0</v>
+      </c>
+      <c r="H42" s="1">
+        <v>0</v>
+      </c>
+      <c r="I42" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K42" s="1">
+        <v>0</v>
+      </c>
+      <c r="V42" s="1">
+        <v>1500</v>
+      </c>
+      <c r="W42" s="1">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="43" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B43" s="1">
+        <v>41</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D43" s="1">
+        <v>14</v>
+      </c>
+      <c r="E43" s="1">
+        <v>2</v>
+      </c>
+      <c r="F43" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G43" s="1">
+        <v>1</v>
+      </c>
+      <c r="H43" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I43" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K43" s="1">
+        <v>210000</v>
+      </c>
+      <c r="V43" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W43" s="1">
+        <v>19</v>
+      </c>
+      <c r="X43" s="2"/>
+    </row>
+    <row r="44" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B44" s="1">
+        <v>42</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="D44" s="1">
+        <v>14</v>
+      </c>
+      <c r="E44" s="1">
+        <v>3</v>
+      </c>
+      <c r="F44" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G44" s="1">
+        <v>2</v>
+      </c>
+      <c r="H44" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K44" s="1">
+        <v>210000</v>
+      </c>
+      <c r="V44" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W44" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="45" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B45" s="1">
+        <v>43</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D45" s="1">
+        <v>14</v>
+      </c>
+      <c r="E45" s="1">
+        <v>4</v>
+      </c>
+      <c r="F45" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G45" s="1">
+        <v>3</v>
+      </c>
+      <c r="H45" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K45" s="1">
+        <v>210000</v>
+      </c>
+      <c r="V45" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W45" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="46" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B46" s="1">
+        <v>44</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D46" s="1">
+        <v>14</v>
+      </c>
+      <c r="E46" s="1">
+        <v>5</v>
+      </c>
+      <c r="F46" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G46" s="1">
+        <v>4</v>
+      </c>
+      <c r="H46" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K46" s="1">
+        <v>210000</v>
+      </c>
+      <c r="V46" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W46" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="47" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B47" s="1">
+        <v>45</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D47" s="1">
+        <v>14</v>
+      </c>
+      <c r="E47" s="1">
+        <v>6</v>
+      </c>
+      <c r="F47" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G47" s="1">
+        <v>5</v>
+      </c>
+      <c r="H47" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="K47" s="1">
+        <v>210000</v>
+      </c>
+      <c r="V47" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W47" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="48" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B48" s="1">
+        <v>46</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D48" s="1">
+        <v>14</v>
+      </c>
+      <c r="E48" s="1">
+        <v>7</v>
+      </c>
+      <c r="F48" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G48" s="1">
+        <v>6</v>
+      </c>
+      <c r="H48" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="K48" s="1">
+        <v>210000</v>
+      </c>
+      <c r="V48" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W48" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="49" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B49" s="1">
+        <v>47</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D49" s="1">
+        <v>14</v>
+      </c>
+      <c r="E49" s="1">
+        <v>8</v>
+      </c>
+      <c r="F49" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G49" s="1">
+        <v>7</v>
+      </c>
+      <c r="H49" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I49" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="K49" s="1">
+        <v>210000</v>
+      </c>
+      <c r="V49" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W49" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B50" s="1">
+        <v>48</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D50" s="1">
+        <v>14</v>
+      </c>
+      <c r="E50" s="1">
+        <v>9</v>
+      </c>
+      <c r="F50" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G50" s="1">
+        <v>8</v>
+      </c>
+      <c r="H50" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I50" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="K50" s="1">
+        <v>210000</v>
+      </c>
+      <c r="V50" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W50" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B51" s="1">
+        <v>49</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D51" s="1">
+        <v>14</v>
+      </c>
+      <c r="E51" s="1">
+        <v>10</v>
+      </c>
+      <c r="F51" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G51" s="1">
+        <v>9</v>
+      </c>
+      <c r="H51" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="K51" s="1">
+        <v>210000</v>
+      </c>
+      <c r="V51" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W51" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="52" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B52" s="1">
+        <v>50</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D52" s="1">
+        <v>14</v>
+      </c>
+      <c r="E52" s="1">
+        <v>11</v>
+      </c>
+      <c r="F52" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G52" s="1">
+        <v>10</v>
+      </c>
+      <c r="H52" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="K52" s="1">
+        <v>210000</v>
+      </c>
+      <c r="V52" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W52" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B53" s="1">
+        <v>51</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53" s="1">
+        <v>14</v>
+      </c>
+      <c r="E53" s="1">
+        <v>12</v>
+      </c>
+      <c r="F53" s="1">
+        <v>2020</v>
+      </c>
+      <c r="G53" s="1">
+        <v>11</v>
+      </c>
+      <c r="H53" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I53" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K53" s="1">
+        <v>210000</v>
+      </c>
+      <c r="V53" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W53" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B54" s="1">
+        <v>52</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D54" s="1">
+        <v>14</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1</v>
+      </c>
+      <c r="F54" s="1">
+        <v>2021</v>
+      </c>
+      <c r="G54" s="1">
+        <v>12</v>
+      </c>
+      <c r="H54" s="1">
+        <v>2021</v>
+      </c>
+      <c r="I54" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J54" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="K54" s="1">
+        <v>210000</v>
+      </c>
+      <c r="V54" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W54" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="55" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B55" s="1">
+        <v>53</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="D55" s="1">
+        <v>15</v>
+      </c>
+      <c r="E55" s="1">
+        <v>10</v>
+      </c>
+      <c r="F55" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G55" s="1">
+        <v>5</v>
+      </c>
+      <c r="H55" s="1">
+        <v>2022</v>
+      </c>
+      <c r="I55" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J55" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="K55" s="1">
+        <v>220800</v>
+      </c>
+      <c r="V55" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W55" s="1">
+        <v>18</v>
+      </c>
+      <c r="X55" s="2"/>
+    </row>
+    <row r="56" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B56" s="1">
+        <v>54</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D56" s="1">
+        <v>15</v>
+      </c>
+      <c r="E56" s="1">
+        <v>5</v>
+      </c>
+      <c r="F56" s="1">
+        <v>2019</v>
+      </c>
+      <c r="G56" s="1">
+        <v>10</v>
+      </c>
+      <c r="H56" s="1">
+        <v>2024</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="K56" s="1">
+        <v>194250</v>
+      </c>
+      <c r="V56" s="1">
+        <v>10000</v>
+      </c>
+      <c r="W56" s="1">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B57" s="1">
+        <v>55</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D57" s="1">
+        <v>15</v>
+      </c>
+      <c r="E57" s="1">
+        <v>10</v>
+      </c>
+      <c r="F57" s="1">
+        <v>2018</v>
+      </c>
+      <c r="G57" s="1">
+        <v>9</v>
+      </c>
+      <c r="H57" s="1">
+        <v>2026</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="K57" s="1">
+        <v>255500</v>
+      </c>
+      <c r="V57" s="1">
+        <v>12000</v>
+      </c>
+      <c r="W57" s="1">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="58" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B58" s="1">
+        <v>56</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D58" s="1">
+        <v>15</v>
+      </c>
+      <c r="E58" s="1">
+        <v>0</v>
+      </c>
+      <c r="F58" s="1">
+        <v>0</v>
+      </c>
+      <c r="G58" s="1">
+        <v>0</v>
+      </c>
+      <c r="H58" s="1">
+        <v>0</v>
+      </c>
+      <c r="I58" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="J58" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="K58" s="1">
+        <v>0</v>
+      </c>
+      <c r="V58" s="1">
+        <v>7500</v>
+      </c>
+      <c r="W58" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="2:24" x14ac:dyDescent="0.35">
+      <c r="B59" s="1">
+        <v>57</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="D59" s="1">
+        <v>16</v>
+      </c>
+      <c r="E59" s="1">
+        <v>6</v>
+      </c>
+      <c r="F59" s="1">
+        <v>2016</v>
+      </c>
+      <c r="G59" s="1">
+        <v>5</v>
+      </c>
+      <c r="H59" s="1">
+        <v>2026</v>
+      </c>
+      <c r="I59" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J59" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="K59" s="1">
+        <v>2100000</v>
+      </c>
+      <c r="V59" s="1">
+        <v>175000</v>
+      </c>
+      <c r="W59" s="1">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -5226,7 +7607,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:D7"/>
   <sheetViews>
@@ -5234,15 +7615,15 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="7.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1">
         <v>0</v>
       </c>
@@ -5256,7 +7637,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B2" t="s">
         <v>7</v>
       </c>
@@ -5267,7 +7648,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>1</v>
       </c>
@@ -5278,7 +7659,7 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>1</v>
       </c>
@@ -5289,7 +7670,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>2</v>
       </c>
@@ -5300,7 +7681,7 @@
         <v>1.4E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>2</v>
       </c>
@@ -5311,7 +7692,7 @@
         <v>1.2999999999999999E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>1</v>
       </c>

</xml_diff>